<commit_message>
feat: tradução da planilha de saída
</commit_message>
<xml_diff>
--- a/public/pdocrud/downloads/file.xlsx
+++ b/public/pdocrud/downloads/file.xlsx
@@ -15,63 +15,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Id sellercentral</t>
-  </si>
-  <si>
-    <t>Id phase</t>
-  </si>
-  <si>
-    <t>Online order number</t>
-  </si>
-  <si>
-    <t>Expected date</t>
-  </si>
-  <si>
-    <t>Isbn</t>
-  </si>
-  <si>
-    <t>Selling price</t>
-  </si>
-  <si>
-    <t>Supplier name</t>
-  </si>
-  <si>
-    <t>Purchase date</t>
-  </si>
-  <si>
-    <t>Ask rating</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+  <si>
+    <t>Nº</t>
+  </si>
+  <si>
+    <t>Endereço verificado</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Canal de Venda</t>
+  </si>
+  <si>
+    <t>Fase do processo</t>
+  </si>
+  <si>
+    <t>ORIGEM</t>
+  </si>
+  <si>
+    <t>Data prevista</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Fornecedor</t>
+  </si>
+  <si>
+    <t>Data da compra</t>
+  </si>
+  <si>
+    <t>Pedir avaliação</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>113-9057255-4699429</t>
+  </si>
+  <si>
+    <t>2022-10-03</t>
   </si>
   <si>
     <t>BR</t>
   </si>
   <si>
-    <t>701-0998366-0286627</t>
-  </si>
-  <si>
-    <t>2022-09-13</t>
-  </si>
-  <si>
-    <t>Janina - BO</t>
-  </si>
-  <si>
-    <t>702-3593699-6443437</t>
-  </si>
-  <si>
-    <t>Janina 103.00</t>
-  </si>
-  <si>
-    <t>701-7788939-7381863</t>
-  </si>
-  <si>
-    <t>2022-09-08</t>
-  </si>
-  <si>
-    <t>2022-08-24</t>
+    <t>702-9539469-6376211</t>
+  </si>
+  <si>
+    <t>2022-09-30</t>
+  </si>
+  <si>
+    <t>701-4234156-8792224</t>
+  </si>
+  <si>
+    <t>2022-10-06</t>
+  </si>
+  <si>
+    <t>701-0432157-5859400</t>
+  </si>
+  <si>
+    <t>701-3702144-9315458</t>
+  </si>
+  <si>
+    <t>701-2876278-8028246</t>
+  </si>
+  <si>
+    <t>701-0629458-5365811</t>
+  </si>
+  <si>
+    <t>111-1946379-8849824</t>
+  </si>
+  <si>
+    <t>702-3181042-6202623</t>
+  </si>
+  <si>
+    <t>702-1869931-7150643</t>
+  </si>
+  <si>
+    <t>702-3400767-2354663</t>
+  </si>
+  <si>
+    <t>701-3308879-0588266</t>
+  </si>
+  <si>
+    <t>113-9220345-5959419</t>
+  </si>
+  <si>
+    <t>2022-10-04</t>
+  </si>
+  <si>
+    <t>701-4807906-0481805</t>
+  </si>
+  <si>
+    <t>702-1837846-6937865</t>
+  </si>
+  <si>
+    <t>113-1749165-3607402</t>
+  </si>
+  <si>
+    <t>2022-10-28</t>
+  </si>
+  <si>
+    <t>702-3059085-2569824</t>
+  </si>
+  <si>
+    <t>701-4339748-7112247</t>
+  </si>
+  <si>
+    <t>701-5615122-7125003</t>
+  </si>
+  <si>
+    <t>702-8166632-3486610</t>
   </si>
 </sst>
 </file>
@@ -410,7 +470,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,7 +478,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -449,98 +509,652 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="0">
-        <v>11596</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>12147</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0">
-        <v>9788568684917</v>
-      </c>
-      <c r="G2" s="0">
-        <v>211.5</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="E2" s="0">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="G2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="0">
+        <v>9788522495689</v>
+      </c>
+      <c r="I2" s="0">
+        <v>80</v>
+      </c>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="0">
-        <v>11613</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12148</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0</v>
       </c>
       <c r="C3" s="0">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="0">
+        <v>9788532510617</v>
+      </c>
+      <c r="I3" s="0">
+        <v>22.5</v>
+      </c>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="0">
+        <v>12149</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0">
+        <v>9788560280728</v>
+      </c>
+      <c r="I4" s="0">
+        <v>187.2</v>
+      </c>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="0">
+        <v>12150</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="0">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="0">
+        <v>9788544238233</v>
+      </c>
+      <c r="I5" s="0">
+        <v>237.6</v>
+      </c>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="0">
+        <v>12151</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="0">
+        <v>9788572444132</v>
+      </c>
+      <c r="I6" s="0">
+        <v>29.7</v>
+      </c>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="0">
+        <v>12152</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="0">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="0">
+        <v>9788516051716</v>
+      </c>
+      <c r="I7" s="0">
+        <v>223.2</v>
+      </c>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="0">
+        <v>12153</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="0">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="0">
+        <v>9788579144387</v>
+      </c>
+      <c r="I8" s="0">
+        <v>297.9</v>
+      </c>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="0">
+        <v>12154</v>
+      </c>
+      <c r="B9" s="0">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="0">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="H9" s="0">
+        <v>9788583930600</v>
+      </c>
+      <c r="I9" s="0">
+        <v>42</v>
+      </c>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="0">
+        <v>12155</v>
+      </c>
+      <c r="B10" s="0">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="0">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="0">
+        <v>9788501403643</v>
+      </c>
+      <c r="I10" s="0">
+        <v>550.8</v>
+      </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="0">
+        <v>12156</v>
+      </c>
+      <c r="B11" s="0">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="0">
+        <v>9788531615245</v>
+      </c>
+      <c r="I11" s="0">
+        <v>45</v>
+      </c>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="0">
+        <v>12157</v>
+      </c>
+      <c r="B12" s="0">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="0">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="0">
+        <v>9788597017236</v>
+      </c>
+      <c r="I12" s="0">
+        <v>729</v>
+      </c>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="0">
+        <v>12158</v>
+      </c>
+      <c r="B13" s="0">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="0">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="0">
+        <v>9788580090666</v>
+      </c>
+      <c r="I13" s="0">
+        <v>43.2</v>
+      </c>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="0">
+        <v>12159</v>
+      </c>
+      <c r="B14" s="0">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="0">
-        <v>9788535203417</v>
-      </c>
-      <c r="G3" s="0">
-        <v>229.5</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="0">
-        <v>11643</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="E14" s="0">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="0">
+        <v>9788501015204</v>
+      </c>
+      <c r="I14" s="0">
+        <v>59</v>
+      </c>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="0">
+        <v>12160</v>
+      </c>
+      <c r="B15" s="0">
+        <v>0</v>
+      </c>
+      <c r="C15" s="0">
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="0">
+        <v>0</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="0">
+        <v>9786559641482</v>
+      </c>
+      <c r="I15" s="0">
+        <v>440.1</v>
+      </c>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+      <c r="L15" s="0"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="0">
+        <v>12161</v>
+      </c>
+      <c r="B16" s="0">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="0">
+        <v>0</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="0">
+        <v>9788580403350</v>
+      </c>
+      <c r="I16" s="0">
+        <v>240.3</v>
+      </c>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
+      <c r="L16" s="0"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="0">
+        <v>12162</v>
+      </c>
+      <c r="B17" s="0">
+        <v>0</v>
+      </c>
+      <c r="C17" s="0">
+        <v>0</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="0">
+        <v>0</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="0">
+        <v>9788556381217</v>
+      </c>
+      <c r="I17" s="0">
+        <v>38</v>
+      </c>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="0">
+        <v>12163</v>
+      </c>
+      <c r="B18" s="0">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="0">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="0">
+        <v>9788577013043</v>
+      </c>
+      <c r="I18" s="0">
+        <v>94.5</v>
+      </c>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="0">
+        <v>12164</v>
+      </c>
+      <c r="B19" s="0">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="0">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="0">
+        <v>9788530986520</v>
+      </c>
+      <c r="I19" s="0">
+        <v>143</v>
+      </c>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="0">
+        <v>12165</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0</v>
+      </c>
+      <c r="C20" s="0">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="0">
+        <v>0</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="0">
-        <v>9788573797114</v>
-      </c>
-      <c r="G4" s="0">
-        <v>515.7</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="0">
-        <v>0</v>
-      </c>
+      <c r="H20" s="0">
+        <v>9788543101392</v>
+      </c>
+      <c r="I20" s="0">
+        <v>51</v>
+      </c>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="0">
+        <v>12166</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0</v>
+      </c>
+      <c r="C21" s="0">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="0">
+        <v>9788577990399</v>
+      </c>
+      <c r="I21" s="0">
+        <v>51</v>
+      </c>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
feat: upload de arquivos para atualização
</commit_message>
<xml_diff>
--- a/public/pdocrud/downloads/file.xlsx
+++ b/public/pdocrud/downloads/file.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
   <si>
     <t>Nº</t>
   </si>
@@ -53,85 +53,274 @@
     <t>Pedir avaliação</t>
   </si>
   <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>701-1209192-6307443</t>
+  </si>
+  <si>
+    <t>2022-10-17</t>
+  </si>
+  <si>
+    <t>701-5391599-9583442</t>
+  </si>
+  <si>
+    <t>701-9461494-3193865</t>
+  </si>
+  <si>
+    <t>2022-10-10</t>
+  </si>
+  <si>
+    <t>701-1423875-1510639</t>
+  </si>
+  <si>
+    <t>701-7893180-7415467</t>
+  </si>
+  <si>
+    <t>701-4662593-4197832</t>
+  </si>
+  <si>
+    <t>701-5775264-6934636</t>
+  </si>
+  <si>
+    <t>702-5526068-5962645</t>
+  </si>
+  <si>
+    <t>701-7493483-1423456</t>
+  </si>
+  <si>
+    <t>701-5293915-9535416</t>
+  </si>
+  <si>
+    <t>702-2963167-6366631</t>
+  </si>
+  <si>
+    <t>702-4090557-3105812</t>
+  </si>
+  <si>
+    <t>701-3223676-8859424</t>
+  </si>
+  <si>
+    <t>702-3127098-8826647</t>
+  </si>
+  <si>
+    <t>702-2653338-7662652</t>
+  </si>
+  <si>
+    <t>702-6459266-5049036</t>
+  </si>
+  <si>
     <t>US</t>
   </si>
   <si>
-    <t>113-9057255-4699429</t>
-  </si>
-  <si>
-    <t>2022-10-03</t>
-  </si>
-  <si>
-    <t>BR</t>
-  </si>
-  <si>
-    <t>702-9539469-6376211</t>
-  </si>
-  <si>
-    <t>2022-09-30</t>
-  </si>
-  <si>
-    <t>701-4234156-8792224</t>
-  </si>
-  <si>
-    <t>2022-10-06</t>
-  </si>
-  <si>
-    <t>701-0432157-5859400</t>
-  </si>
-  <si>
-    <t>701-3702144-9315458</t>
-  </si>
-  <si>
-    <t>701-2876278-8028246</t>
-  </si>
-  <si>
-    <t>701-0629458-5365811</t>
-  </si>
-  <si>
-    <t>111-1946379-8849824</t>
-  </si>
-  <si>
-    <t>702-3181042-6202623</t>
-  </si>
-  <si>
-    <t>702-1869931-7150643</t>
-  </si>
-  <si>
-    <t>702-3400767-2354663</t>
-  </si>
-  <si>
-    <t>701-3308879-0588266</t>
-  </si>
-  <si>
-    <t>113-9220345-5959419</t>
-  </si>
-  <si>
-    <t>2022-10-04</t>
-  </si>
-  <si>
-    <t>701-4807906-0481805</t>
-  </si>
-  <si>
-    <t>702-1837846-6937865</t>
-  </si>
-  <si>
-    <t>113-1749165-3607402</t>
-  </si>
-  <si>
-    <t>2022-10-28</t>
-  </si>
-  <si>
-    <t>702-3059085-2569824</t>
-  </si>
-  <si>
-    <t>701-4339748-7112247</t>
-  </si>
-  <si>
-    <t>701-5615122-7125003</t>
-  </si>
-  <si>
-    <t>702-8166632-3486610</t>
+    <t>113-8137802-5444221</t>
+  </si>
+  <si>
+    <t>2022-11-07</t>
+  </si>
+  <si>
+    <t>701-2605761-1778604</t>
+  </si>
+  <si>
+    <t>702-4734067-9853868</t>
+  </si>
+  <si>
+    <t>701-4675306-2159426</t>
+  </si>
+  <si>
+    <t>702-8581848-5065867</t>
+  </si>
+  <si>
+    <t>701-1081896-4552200</t>
+  </si>
+  <si>
+    <t>701-0398557-7225030</t>
+  </si>
+  <si>
+    <t>702-6412282-6492252</t>
+  </si>
+  <si>
+    <t>701-9441835-8365027</t>
+  </si>
+  <si>
+    <t>702-0541042-7986612</t>
+  </si>
+  <si>
+    <t>701-2774317-8808253</t>
+  </si>
+  <si>
+    <t>701-6714138-2493032</t>
+  </si>
+  <si>
+    <t>701-5820993-4525858</t>
+  </si>
+  <si>
+    <t>702-1371093-4160222</t>
+  </si>
+  <si>
+    <t>702-6429587-6356255</t>
+  </si>
+  <si>
+    <t>702-3154588-7526647</t>
+  </si>
+  <si>
+    <t>701-1935748-4582646</t>
+  </si>
+  <si>
+    <t>702-6244304-2801803</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>701-1580357-9105839</t>
+  </si>
+  <si>
+    <t>2022-11-08</t>
+  </si>
+  <si>
+    <t>702-4319804-1909063</t>
+  </si>
+  <si>
+    <t>701-6180967-0748219</t>
+  </si>
+  <si>
+    <t>702-2860534-4951409</t>
+  </si>
+  <si>
+    <t>701-1056413-0229820</t>
+  </si>
+  <si>
+    <t>701-6369273-9421046</t>
+  </si>
+  <si>
+    <t>701-9976800-4362654</t>
+  </si>
+  <si>
+    <t>702-5084301-3141067</t>
+  </si>
+  <si>
+    <t>702-1007666-4930622</t>
+  </si>
+  <si>
+    <t>702-7303982-1342657</t>
+  </si>
+  <si>
+    <t>701-7187841-0541022</t>
+  </si>
+  <si>
+    <t>702-1956965-6965062</t>
+  </si>
+  <si>
+    <t>702-5960361-3817816</t>
+  </si>
+  <si>
+    <t>701-6560153-4031461</t>
+  </si>
+  <si>
+    <t>701-5283875-4744257</t>
+  </si>
+  <si>
+    <t>701-7000366-9801049</t>
+  </si>
+  <si>
+    <t>702-1474427-3393039</t>
+  </si>
+  <si>
+    <t>702-3494985-0964218</t>
+  </si>
+  <si>
+    <t>701-4376754-9769800</t>
+  </si>
+  <si>
+    <t>702-3331615-1770624</t>
+  </si>
+  <si>
+    <t>702-8864712-0677844</t>
+  </si>
+  <si>
+    <t>702-7945653-1627415</t>
+  </si>
+  <si>
+    <t>702-2176046-8541054</t>
+  </si>
+  <si>
+    <t>702-3620970-5012201</t>
+  </si>
+  <si>
+    <t>701-0592148-9426661</t>
+  </si>
+  <si>
+    <t>702-9244063-0976253</t>
+  </si>
+  <si>
+    <t>702-2058268-2175411</t>
+  </si>
+  <si>
+    <t>702-6654138-6794611</t>
+  </si>
+  <si>
+    <t>701-0140848-0867453</t>
+  </si>
+  <si>
+    <t>702-7673869-9285807</t>
+  </si>
+  <si>
+    <t>701-7600192-1835446</t>
+  </si>
+  <si>
+    <t>701-5120795-3460251</t>
+  </si>
+  <si>
+    <t>702-3824538-1708264</t>
+  </si>
+  <si>
+    <t>702-5431481-8183461</t>
+  </si>
+  <si>
+    <t>701-7154317-1124224</t>
+  </si>
+  <si>
+    <t>701-9008725-3339420</t>
+  </si>
+  <si>
+    <t>701-2313265-9166657</t>
+  </si>
+  <si>
+    <t>702-4367131-3214669</t>
+  </si>
+  <si>
+    <t>702-2154948-3252256</t>
+  </si>
+  <si>
+    <t>702-5526123-5562660</t>
+  </si>
+  <si>
+    <t>702-2672290-7623402</t>
+  </si>
+  <si>
+    <t>702-0551478-1147421</t>
+  </si>
+  <si>
+    <t>702-9588226-6843425</t>
+  </si>
+  <si>
+    <t>702-0522937-4361011</t>
+  </si>
+  <si>
+    <t>701-4446158-9705043</t>
+  </si>
+  <si>
+    <t>702-3448042-2531437</t>
+  </si>
+  <si>
+    <t>2022-10-11</t>
+  </si>
+  <si>
+    <t>701-5400778-0580268</t>
+  </si>
+  <si>
+    <t>702-2711942-9791437</t>
   </si>
 </sst>
 </file>
@@ -470,7 +659,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,7 +707,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="0">
-        <v>12147</v>
+        <v>12348</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -539,10 +728,10 @@
         <v>14</v>
       </c>
       <c r="H2" s="0">
-        <v>9788522495689</v>
+        <v>9788586584022</v>
       </c>
       <c r="I2" s="0">
-        <v>80</v>
+        <v>79.05</v>
       </c>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
@@ -550,7 +739,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="0">
-        <v>12148</v>
+        <v>12349</v>
       </c>
       <c r="B3" s="0">
         <v>0</v>
@@ -559,22 +748,22 @@
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0">
-        <v>9788532510617</v>
+        <v>9788583000044</v>
       </c>
       <c r="I3" s="0">
-        <v>22.5</v>
+        <v>151.59</v>
       </c>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
@@ -582,7 +771,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="0">
-        <v>12149</v>
+        <v>12350</v>
       </c>
       <c r="B4" s="0">
         <v>0</v>
@@ -591,22 +780,22 @@
         <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0">
         <v>0</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" s="0">
-        <v>9788560280728</v>
+        <v>9788580408935</v>
       </c>
       <c r="I4" s="0">
-        <v>187.2</v>
+        <v>255.75</v>
       </c>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
@@ -614,7 +803,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="0">
-        <v>12150</v>
+        <v>12351</v>
       </c>
       <c r="B5" s="0">
         <v>0</v>
@@ -623,22 +812,22 @@
         <v>0</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" s="0">
-        <v>9788544238233</v>
+        <v>9788522470716</v>
       </c>
       <c r="I5" s="0">
-        <v>237.6</v>
+        <v>156.24</v>
       </c>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
@@ -646,7 +835,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="0">
-        <v>12151</v>
+        <v>12352</v>
       </c>
       <c r="B6" s="0">
         <v>0</v>
@@ -655,22 +844,22 @@
         <v>0</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0">
         <v>0</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H6" s="0">
-        <v>9788572444132</v>
+        <v>9780857625410</v>
       </c>
       <c r="I6" s="0">
-        <v>29.7</v>
+        <v>154.38</v>
       </c>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
@@ -678,7 +867,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="0">
-        <v>12152</v>
+        <v>12353</v>
       </c>
       <c r="B7" s="0">
         <v>0</v>
@@ -687,22 +876,22 @@
         <v>0</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0">
         <v>0</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H7" s="0">
-        <v>9788516051716</v>
+        <v>9788533604858</v>
       </c>
       <c r="I7" s="0">
-        <v>223.2</v>
+        <v>69.75</v>
       </c>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
@@ -710,7 +899,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="0">
-        <v>12153</v>
+        <v>12354</v>
       </c>
       <c r="B8" s="0">
         <v>0</v>
@@ -719,22 +908,22 @@
         <v>0</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0">
         <v>0</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H8" s="0">
-        <v>9788579144387</v>
+        <v>9788582604953</v>
       </c>
       <c r="I8" s="0">
-        <v>297.9</v>
+        <v>275.28</v>
       </c>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
@@ -742,7 +931,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="0">
-        <v>12154</v>
+        <v>12355</v>
       </c>
       <c r="B9" s="0">
         <v>0</v>
@@ -757,16 +946,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H9" s="0">
-        <v>9788583930600</v>
+        <v>9788535903454</v>
       </c>
       <c r="I9" s="0">
-        <v>42</v>
+        <v>57.66</v>
       </c>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
@@ -774,7 +963,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="0">
-        <v>12155</v>
+        <v>12356</v>
       </c>
       <c r="B10" s="0">
         <v>0</v>
@@ -783,22 +972,22 @@
         <v>0</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0">
         <v>0</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H10" s="0">
-        <v>9788501403643</v>
+        <v>9788516051716</v>
       </c>
       <c r="I10" s="0">
-        <v>550.8</v>
+        <v>130.2</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -806,7 +995,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="0">
-        <v>12156</v>
+        <v>12357</v>
       </c>
       <c r="B11" s="0">
         <v>0</v>
@@ -815,22 +1004,22 @@
         <v>0</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0">
         <v>0</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H11" s="0">
-        <v>9788531615245</v>
+        <v>7895377000677</v>
       </c>
       <c r="I11" s="0">
-        <v>45</v>
+        <v>232.5</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
@@ -838,7 +1027,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="0">
-        <v>12157</v>
+        <v>12358</v>
       </c>
       <c r="B12" s="0">
         <v>0</v>
@@ -847,22 +1036,22 @@
         <v>0</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0">
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="0">
-        <v>9788597017236</v>
+        <v>9788534921961</v>
       </c>
       <c r="I12" s="0">
-        <v>729</v>
+        <v>243.66</v>
       </c>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -870,7 +1059,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="0">
-        <v>12158</v>
+        <v>12359</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
@@ -879,22 +1068,22 @@
         <v>0</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0">
         <v>0</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H13" s="0">
-        <v>9788580090666</v>
+        <v>9788565985260</v>
       </c>
       <c r="I13" s="0">
-        <v>43.2</v>
+        <v>163.68</v>
       </c>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -902,7 +1091,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="0">
-        <v>12159</v>
+        <v>12360</v>
       </c>
       <c r="B14" s="0">
         <v>0</v>
@@ -917,16 +1106,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H14" s="0">
-        <v>9788501015204</v>
+        <v>9788530983178</v>
       </c>
       <c r="I14" s="0">
-        <v>59</v>
+        <v>323.64</v>
       </c>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -934,7 +1123,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="0">
-        <v>12160</v>
+        <v>12361</v>
       </c>
       <c r="B15" s="0">
         <v>0</v>
@@ -943,22 +1132,22 @@
         <v>0</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E15" s="0">
         <v>0</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H15" s="0">
-        <v>9786559641482</v>
+        <v>9788551804247</v>
       </c>
       <c r="I15" s="0">
-        <v>440.1</v>
+        <v>92.07</v>
       </c>
       <c r="J15" s="0"/>
       <c r="K15" s="0"/>
@@ -966,7 +1155,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="0">
-        <v>12161</v>
+        <v>12362</v>
       </c>
       <c r="B16" s="0">
         <v>0</v>
@@ -975,22 +1164,22 @@
         <v>0</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0">
         <v>0</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H16" s="0">
-        <v>9788580403350</v>
+        <v>9788544237793</v>
       </c>
       <c r="I16" s="0">
-        <v>240.3</v>
+        <v>446.4</v>
       </c>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
@@ -998,7 +1187,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="0">
-        <v>12162</v>
+        <v>12363</v>
       </c>
       <c r="B17" s="0">
         <v>0</v>
@@ -1013,16 +1202,16 @@
         <v>0</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="H17" s="0">
-        <v>9788556381217</v>
+        <v>9788577010585</v>
       </c>
       <c r="I17" s="0">
-        <v>38</v>
+        <v>130.2</v>
       </c>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -1030,7 +1219,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="0">
-        <v>12163</v>
+        <v>12364</v>
       </c>
       <c r="B18" s="0">
         <v>0</v>
@@ -1039,22 +1228,22 @@
         <v>0</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="E18" s="0">
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H18" s="0">
-        <v>9788577013043</v>
+        <v>9788580092813</v>
       </c>
       <c r="I18" s="0">
-        <v>94.5</v>
+        <v>130.2</v>
       </c>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -1062,31 +1251,31 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="0">
-        <v>12164</v>
+        <v>12365</v>
       </c>
       <c r="B19" s="0">
         <v>0</v>
       </c>
       <c r="C19" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0">
         <v>0</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H19" s="0">
-        <v>9788530986520</v>
+        <v>9788535287158</v>
       </c>
       <c r="I19" s="0">
-        <v>143</v>
+        <v>401.76</v>
       </c>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
@@ -1094,31 +1283,31 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="0">
-        <v>12165</v>
+        <v>12366</v>
       </c>
       <c r="B20" s="0">
         <v>0</v>
       </c>
       <c r="C20" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0">
         <v>0</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H20" s="0">
-        <v>9788543101392</v>
+        <v>9788576089742</v>
       </c>
       <c r="I20" s="0">
-        <v>51</v>
+        <v>140.43</v>
       </c>
       <c r="J20" s="0"/>
       <c r="K20" s="0"/>
@@ -1126,35 +1315,2019 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="0">
-        <v>12166</v>
+        <v>12367</v>
       </c>
       <c r="B21" s="0">
         <v>0</v>
       </c>
       <c r="C21" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0">
         <v>0</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H21" s="0">
-        <v>9788577990399</v>
+        <v>9788583100195</v>
       </c>
       <c r="I21" s="0">
-        <v>51</v>
+        <v>269.7</v>
       </c>
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
       <c r="L21" s="0"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="0">
+        <v>12368</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="0">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="0">
+        <v>9788581301570</v>
+      </c>
+      <c r="I22" s="0">
+        <v>111.6</v>
+      </c>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="0">
+        <v>12369</v>
+      </c>
+      <c r="B23" s="0">
+        <v>0</v>
+      </c>
+      <c r="C23" s="0">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="0">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="0">
+        <v>9786586093377</v>
+      </c>
+      <c r="I23" s="0">
+        <v>141.36</v>
+      </c>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="0">
+        <v>12370</v>
+      </c>
+      <c r="B24" s="0">
+        <v>0</v>
+      </c>
+      <c r="C24" s="0">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="0">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="0">
+        <v>9788578542061</v>
+      </c>
+      <c r="I24" s="0">
+        <v>122.76</v>
+      </c>
+      <c r="J24" s="0"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="0"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="0">
+        <v>12371</v>
+      </c>
+      <c r="B25" s="0">
+        <v>0</v>
+      </c>
+      <c r="C25" s="0">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="0">
+        <v>0</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="0">
+        <v>9788502636293</v>
+      </c>
+      <c r="I25" s="0">
+        <v>146.94</v>
+      </c>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="0">
+        <v>12372</v>
+      </c>
+      <c r="B26" s="0">
+        <v>0</v>
+      </c>
+      <c r="C26" s="0">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="0">
+        <v>0</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="0">
+        <v>9788531611292</v>
+      </c>
+      <c r="I26" s="0">
+        <v>102.3</v>
+      </c>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="0">
+        <v>12373</v>
+      </c>
+      <c r="B27" s="0">
+        <v>0</v>
+      </c>
+      <c r="C27" s="0">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="0">
+        <v>0</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="0">
+        <v>9788545006046</v>
+      </c>
+      <c r="I27" s="0">
+        <v>226.92</v>
+      </c>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="0">
+        <v>12374</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="0">
+        <v>0</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="0">
+        <v>9788535919714</v>
+      </c>
+      <c r="I28" s="0">
+        <v>88.35</v>
+      </c>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="0">
+        <v>12375</v>
+      </c>
+      <c r="B29" s="0">
+        <v>0</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="0">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="0">
+        <v>9788577893515</v>
+      </c>
+      <c r="I29" s="0">
+        <v>171.12</v>
+      </c>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="0">
+        <v>12376</v>
+      </c>
+      <c r="B30" s="0">
+        <v>0</v>
+      </c>
+      <c r="C30" s="0">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="0">
+        <v>0</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="0">
+        <v>9788561467166</v>
+      </c>
+      <c r="I30" s="0">
+        <v>93.93</v>
+      </c>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="0">
+        <v>12377</v>
+      </c>
+      <c r="B31" s="0">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="0">
+        <v>0</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="0">
+        <v>9788578542238</v>
+      </c>
+      <c r="I31" s="0">
+        <v>133.92</v>
+      </c>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="0">
+        <v>12378</v>
+      </c>
+      <c r="B32" s="0">
+        <v>0</v>
+      </c>
+      <c r="C32" s="0">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="0">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="0">
+        <v>9788554085018</v>
+      </c>
+      <c r="I32" s="0">
+        <v>353.4</v>
+      </c>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="0">
+        <v>12379</v>
+      </c>
+      <c r="B33" s="0">
+        <v>0</v>
+      </c>
+      <c r="C33" s="0">
+        <v>0</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="0">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="0">
+        <v>9788578230753</v>
+      </c>
+      <c r="I33" s="0">
+        <v>96.72</v>
+      </c>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="0">
+        <v>12380</v>
+      </c>
+      <c r="B34" s="0">
+        <v>0</v>
+      </c>
+      <c r="C34" s="0">
+        <v>0</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="0">
+        <v>0</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="0">
+        <v>9788594540416</v>
+      </c>
+      <c r="I34" s="0">
+        <v>130.2</v>
+      </c>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="0">
+        <v>12381</v>
+      </c>
+      <c r="B35" s="0">
+        <v>0</v>
+      </c>
+      <c r="C35" s="0">
+        <v>0</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="0">
+        <v>0</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="0">
+        <v>9788575033890</v>
+      </c>
+      <c r="I35" s="0">
+        <v>75.33</v>
+      </c>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="0">
+        <v>12382</v>
+      </c>
+      <c r="B36" s="0">
+        <v>0</v>
+      </c>
+      <c r="C36" s="0">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="0">
+        <v>0</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H36" s="0">
+        <v>9788547310288</v>
+      </c>
+      <c r="I36" s="0">
+        <v>56</v>
+      </c>
+      <c r="J36" s="0"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="0">
+        <v>12383</v>
+      </c>
+      <c r="B37" s="0">
+        <v>0</v>
+      </c>
+      <c r="C37" s="0">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="0">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="0">
+        <v>9788503011082</v>
+      </c>
+      <c r="I37" s="0">
+        <v>130.2</v>
+      </c>
+      <c r="J37" s="0"/>
+      <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="0">
+        <v>12384</v>
+      </c>
+      <c r="B38" s="0">
+        <v>0</v>
+      </c>
+      <c r="C38" s="0">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="0">
+        <v>0</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="0">
+        <v>9788538810292</v>
+      </c>
+      <c r="I38" s="0">
+        <v>265.98</v>
+      </c>
+      <c r="J38" s="0"/>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="0">
+        <v>12385</v>
+      </c>
+      <c r="B39" s="0">
+        <v>0</v>
+      </c>
+      <c r="C39" s="0">
+        <v>0</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="0">
+        <v>0</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="0">
+        <v>9788520942215</v>
+      </c>
+      <c r="I39" s="0">
+        <v>334.8</v>
+      </c>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="0">
+        <v>12386</v>
+      </c>
+      <c r="B40" s="0">
+        <v>0</v>
+      </c>
+      <c r="C40" s="0">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="0">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" s="0">
+        <v>9788535909432</v>
+      </c>
+      <c r="I40" s="0">
+        <v>74.4</v>
+      </c>
+      <c r="J40" s="0"/>
+      <c r="K40" s="0"/>
+      <c r="L40" s="0"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="0">
+        <v>12387</v>
+      </c>
+      <c r="B41" s="0">
+        <v>0</v>
+      </c>
+      <c r="C41" s="0">
+        <v>0</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="0">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="0">
+        <v>9788573255515</v>
+      </c>
+      <c r="I41" s="0">
+        <v>70.68</v>
+      </c>
+      <c r="J41" s="0"/>
+      <c r="K41" s="0"/>
+      <c r="L41" s="0"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="0">
+        <v>12388</v>
+      </c>
+      <c r="B42" s="0">
+        <v>0</v>
+      </c>
+      <c r="C42" s="0">
+        <v>0</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="0">
+        <v>0</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="0">
+        <v>9788576170464</v>
+      </c>
+      <c r="I42" s="0">
+        <v>66.96</v>
+      </c>
+      <c r="J42" s="0"/>
+      <c r="K42" s="0"/>
+      <c r="L42" s="0"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="0">
+        <v>12389</v>
+      </c>
+      <c r="B43" s="0">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0">
+        <v>0</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="0">
+        <v>0</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="0">
+        <v>9788577852673</v>
+      </c>
+      <c r="I43" s="0">
+        <v>88.35</v>
+      </c>
+      <c r="J43" s="0"/>
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="0">
+        <v>12390</v>
+      </c>
+      <c r="B44" s="0">
+        <v>0</v>
+      </c>
+      <c r="C44" s="0">
+        <v>0</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="0">
+        <v>0</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="0">
+        <v>9788535919714</v>
+      </c>
+      <c r="I44" s="0">
+        <v>88.35</v>
+      </c>
+      <c r="J44" s="0"/>
+      <c r="K44" s="0"/>
+      <c r="L44" s="0"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="0">
+        <v>12391</v>
+      </c>
+      <c r="B45" s="0">
+        <v>0</v>
+      </c>
+      <c r="C45" s="0">
+        <v>0</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="0">
+        <v>0</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="0">
+        <v>9788527727631</v>
+      </c>
+      <c r="I45" s="0">
+        <v>671.46</v>
+      </c>
+      <c r="J45" s="0"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="0">
+        <v>12392</v>
+      </c>
+      <c r="B46" s="0">
+        <v>0</v>
+      </c>
+      <c r="C46" s="0">
+        <v>0</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="0">
+        <v>0</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="0">
+        <v>9788582424056</v>
+      </c>
+      <c r="I46" s="0">
+        <v>221.34</v>
+      </c>
+      <c r="J46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="0">
+        <v>12393</v>
+      </c>
+      <c r="B47" s="0">
+        <v>0</v>
+      </c>
+      <c r="C47" s="0">
+        <v>0</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="0">
+        <v>0</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="0">
+        <v>9788581744209</v>
+      </c>
+      <c r="I47" s="0">
+        <v>254.82</v>
+      </c>
+      <c r="J47" s="0"/>
+      <c r="K47" s="0"/>
+      <c r="L47" s="0"/>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="0">
+        <v>12394</v>
+      </c>
+      <c r="B48" s="0">
+        <v>0</v>
+      </c>
+      <c r="C48" s="0">
+        <v>0</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="0">
+        <v>0</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="0">
+        <v>9788595010154</v>
+      </c>
+      <c r="I48" s="0">
+        <v>252.96</v>
+      </c>
+      <c r="J48" s="0"/>
+      <c r="K48" s="0"/>
+      <c r="L48" s="0"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="0">
+        <v>12395</v>
+      </c>
+      <c r="B49" s="0">
+        <v>0</v>
+      </c>
+      <c r="C49" s="0">
+        <v>0</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="0">
+        <v>0</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="0">
+        <v>9788576651703</v>
+      </c>
+      <c r="I49" s="0">
+        <v>74.4</v>
+      </c>
+      <c r="J49" s="0"/>
+      <c r="K49" s="0"/>
+      <c r="L49" s="0"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="0">
+        <v>12396</v>
+      </c>
+      <c r="B50" s="0">
+        <v>0</v>
+      </c>
+      <c r="C50" s="0">
+        <v>0</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="0">
+        <v>0</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" s="0">
+        <v>9788531406119</v>
+      </c>
+      <c r="I50" s="0">
+        <v>156.24</v>
+      </c>
+      <c r="J50" s="0"/>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="0">
+        <v>12397</v>
+      </c>
+      <c r="B51" s="0">
+        <v>0</v>
+      </c>
+      <c r="C51" s="0">
+        <v>0</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="0">
+        <v>0</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H51" s="0">
+        <v>9788579144189</v>
+      </c>
+      <c r="I51" s="0">
+        <v>102.3</v>
+      </c>
+      <c r="J51" s="0"/>
+      <c r="K51" s="0"/>
+      <c r="L51" s="0"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="0">
+        <v>12398</v>
+      </c>
+      <c r="B52" s="0">
+        <v>0</v>
+      </c>
+      <c r="C52" s="0">
+        <v>0</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="0">
+        <v>0</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="0">
+        <v>9788587199096</v>
+      </c>
+      <c r="I52" s="0">
+        <v>79.05</v>
+      </c>
+      <c r="J52" s="0"/>
+      <c r="K52" s="0"/>
+      <c r="L52" s="0"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="0">
+        <v>12399</v>
+      </c>
+      <c r="B53" s="0">
+        <v>0</v>
+      </c>
+      <c r="C53" s="0">
+        <v>0</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="0">
+        <v>0</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H53" s="0">
+        <v>9788538802846</v>
+      </c>
+      <c r="I53" s="0">
+        <v>583.11</v>
+      </c>
+      <c r="J53" s="0"/>
+      <c r="K53" s="0"/>
+      <c r="L53" s="0"/>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="0">
+        <v>12400</v>
+      </c>
+      <c r="B54" s="0">
+        <v>0</v>
+      </c>
+      <c r="C54" s="0">
+        <v>0</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="0">
+        <v>0</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="0">
+        <v>9786556059914</v>
+      </c>
+      <c r="I54" s="0">
+        <v>170.19</v>
+      </c>
+      <c r="J54" s="0"/>
+      <c r="K54" s="0"/>
+      <c r="L54" s="0"/>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="0">
+        <v>12401</v>
+      </c>
+      <c r="B55" s="0">
+        <v>0</v>
+      </c>
+      <c r="C55" s="0">
+        <v>0</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" s="0">
+        <v>0</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="0">
+        <v>9788575326169</v>
+      </c>
+      <c r="I55" s="0">
+        <v>140.43</v>
+      </c>
+      <c r="J55" s="0"/>
+      <c r="K55" s="0"/>
+      <c r="L55" s="0"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="0">
+        <v>12402</v>
+      </c>
+      <c r="B56" s="0">
+        <v>0</v>
+      </c>
+      <c r="C56" s="0">
+        <v>0</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="0">
+        <v>0</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="0">
+        <v>9788581496771</v>
+      </c>
+      <c r="I56" s="0">
+        <v>134.85</v>
+      </c>
+      <c r="J56" s="0"/>
+      <c r="K56" s="0"/>
+      <c r="L56" s="0"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="0">
+        <v>12403</v>
+      </c>
+      <c r="B57" s="0">
+        <v>0</v>
+      </c>
+      <c r="C57" s="0">
+        <v>0</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="0">
+        <v>0</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="0">
+        <v>9788567861289</v>
+      </c>
+      <c r="I57" s="0">
+        <v>152.52</v>
+      </c>
+      <c r="J57" s="0"/>
+      <c r="K57" s="0"/>
+      <c r="L57" s="0"/>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="0">
+        <v>12404</v>
+      </c>
+      <c r="B58" s="0">
+        <v>0</v>
+      </c>
+      <c r="C58" s="0">
+        <v>0</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="0">
+        <v>0</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="0">
+        <v>9788532510136</v>
+      </c>
+      <c r="I58" s="0">
+        <v>110.67</v>
+      </c>
+      <c r="J58" s="0"/>
+      <c r="K58" s="0"/>
+      <c r="L58" s="0"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="0">
+        <v>12405</v>
+      </c>
+      <c r="B59" s="0">
+        <v>0</v>
+      </c>
+      <c r="C59" s="0">
+        <v>0</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E59" s="0">
+        <v>0</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="0">
+        <v>9788532528575</v>
+      </c>
+      <c r="I59" s="0">
+        <v>88.35</v>
+      </c>
+      <c r="J59" s="0"/>
+      <c r="K59" s="0"/>
+      <c r="L59" s="0"/>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="0">
+        <v>12406</v>
+      </c>
+      <c r="B60" s="0">
+        <v>0</v>
+      </c>
+      <c r="C60" s="0">
+        <v>0</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="0">
+        <v>0</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H60" s="0">
+        <v>9788569538042</v>
+      </c>
+      <c r="I60" s="0">
+        <v>135.78</v>
+      </c>
+      <c r="J60" s="0"/>
+      <c r="K60" s="0"/>
+      <c r="L60" s="0"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="0">
+        <v>12407</v>
+      </c>
+      <c r="B61" s="0">
+        <v>0</v>
+      </c>
+      <c r="C61" s="0">
+        <v>0</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="0">
+        <v>0</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="0">
+        <v>9788535911282</v>
+      </c>
+      <c r="I61" s="0">
+        <v>213.9</v>
+      </c>
+      <c r="J61" s="0"/>
+      <c r="K61" s="0"/>
+      <c r="L61" s="0"/>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="0">
+        <v>12408</v>
+      </c>
+      <c r="B62" s="0">
+        <v>0</v>
+      </c>
+      <c r="C62" s="0">
+        <v>0</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="0">
+        <v>0</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" s="0">
+        <v>9789723016734</v>
+      </c>
+      <c r="I62" s="0">
+        <v>123.69</v>
+      </c>
+      <c r="J62" s="0"/>
+      <c r="K62" s="0"/>
+      <c r="L62" s="0"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="0">
+        <v>12409</v>
+      </c>
+      <c r="B63" s="0">
+        <v>0</v>
+      </c>
+      <c r="C63" s="0">
+        <v>0</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="0">
+        <v>0</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="0">
+        <v>9788539608683</v>
+      </c>
+      <c r="I63" s="0">
+        <v>132.99</v>
+      </c>
+      <c r="J63" s="0"/>
+      <c r="K63" s="0"/>
+      <c r="L63" s="0"/>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="0">
+        <v>12410</v>
+      </c>
+      <c r="B64" s="0">
+        <v>0</v>
+      </c>
+      <c r="C64" s="0">
+        <v>0</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" s="0">
+        <v>0</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H64" s="0">
+        <v>9788580632040</v>
+      </c>
+      <c r="I64" s="0">
+        <v>73.47</v>
+      </c>
+      <c r="J64" s="0"/>
+      <c r="K64" s="0"/>
+      <c r="L64" s="0"/>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="0">
+        <v>12411</v>
+      </c>
+      <c r="B65" s="0">
+        <v>0</v>
+      </c>
+      <c r="C65" s="0">
+        <v>0</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="0">
+        <v>0</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" s="0">
+        <v>9788522450572</v>
+      </c>
+      <c r="I65" s="0">
+        <v>306.9</v>
+      </c>
+      <c r="J65" s="0"/>
+      <c r="K65" s="0"/>
+      <c r="L65" s="0"/>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="0">
+        <v>12412</v>
+      </c>
+      <c r="B66" s="0">
+        <v>0</v>
+      </c>
+      <c r="C66" s="0">
+        <v>0</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="0">
+        <v>0</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="0">
+        <v>9788577001200</v>
+      </c>
+      <c r="I66" s="0">
+        <v>165.54</v>
+      </c>
+      <c r="J66" s="0"/>
+      <c r="K66" s="0"/>
+      <c r="L66" s="0"/>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="0">
+        <v>12413</v>
+      </c>
+      <c r="B67" s="0">
+        <v>0</v>
+      </c>
+      <c r="C67" s="0">
+        <v>0</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="0">
+        <v>0</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" s="0">
+        <v>9788574124032</v>
+      </c>
+      <c r="I67" s="0">
+        <v>95.79</v>
+      </c>
+      <c r="J67" s="0"/>
+      <c r="K67" s="0"/>
+      <c r="L67" s="0"/>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="0">
+        <v>12414</v>
+      </c>
+      <c r="B68" s="0">
+        <v>0</v>
+      </c>
+      <c r="C68" s="0">
+        <v>0</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="0">
+        <v>0</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="0">
+        <v>7898572200972</v>
+      </c>
+      <c r="I68" s="0">
+        <v>244.59</v>
+      </c>
+      <c r="J68" s="0"/>
+      <c r="K68" s="0"/>
+      <c r="L68" s="0"/>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="0">
+        <v>12415</v>
+      </c>
+      <c r="B69" s="0">
+        <v>0</v>
+      </c>
+      <c r="C69" s="0">
+        <v>0</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="0">
+        <v>0</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" s="0">
+        <v>9788594660619</v>
+      </c>
+      <c r="I69" s="0">
+        <v>96.72</v>
+      </c>
+      <c r="J69" s="0"/>
+      <c r="K69" s="0"/>
+      <c r="L69" s="0"/>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="0">
+        <v>12416</v>
+      </c>
+      <c r="B70" s="0">
+        <v>0</v>
+      </c>
+      <c r="C70" s="0">
+        <v>0</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="0">
+        <v>0</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70" s="0">
+        <v>9788537010532</v>
+      </c>
+      <c r="I70" s="0">
+        <v>93</v>
+      </c>
+      <c r="J70" s="0"/>
+      <c r="K70" s="0"/>
+      <c r="L70" s="0"/>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="0">
+        <v>12417</v>
+      </c>
+      <c r="B71" s="0">
+        <v>0</v>
+      </c>
+      <c r="C71" s="0">
+        <v>0</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="0">
+        <v>0</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="0">
+        <v>9788504020311</v>
+      </c>
+      <c r="I71" s="0">
+        <v>98.58</v>
+      </c>
+      <c r="J71" s="0"/>
+      <c r="K71" s="0"/>
+      <c r="L71" s="0"/>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="0">
+        <v>12418</v>
+      </c>
+      <c r="B72" s="0">
+        <v>0</v>
+      </c>
+      <c r="C72" s="0">
+        <v>0</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="0">
+        <v>0</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72" s="0">
+        <v>9788535247633</v>
+      </c>
+      <c r="I72" s="0">
+        <v>176.7</v>
+      </c>
+      <c r="J72" s="0"/>
+      <c r="K72" s="0"/>
+      <c r="L72" s="0"/>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="0">
+        <v>12419</v>
+      </c>
+      <c r="B73" s="0">
+        <v>0</v>
+      </c>
+      <c r="C73" s="0">
+        <v>0</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="0">
+        <v>0</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H73" s="0">
+        <v>9788562219146</v>
+      </c>
+      <c r="I73" s="0">
+        <v>82.77</v>
+      </c>
+      <c r="J73" s="0"/>
+      <c r="K73" s="0"/>
+      <c r="L73" s="0"/>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="0">
+        <v>12420</v>
+      </c>
+      <c r="B74" s="0">
+        <v>0</v>
+      </c>
+      <c r="C74" s="0">
+        <v>0</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74" s="0">
+        <v>0</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="0">
+        <v>9786558693567</v>
+      </c>
+      <c r="I74" s="0">
+        <v>88.35</v>
+      </c>
+      <c r="J74" s="0"/>
+      <c r="K74" s="0"/>
+      <c r="L74" s="0"/>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="0">
+        <v>12421</v>
+      </c>
+      <c r="B75" s="0">
+        <v>0</v>
+      </c>
+      <c r="C75" s="0">
+        <v>0</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="0">
+        <v>0</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H75" s="0">
+        <v>9788522511471</v>
+      </c>
+      <c r="I75" s="0">
+        <v>87.42</v>
+      </c>
+      <c r="J75" s="0"/>
+      <c r="K75" s="0"/>
+      <c r="L75" s="0"/>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="0">
+        <v>12422</v>
+      </c>
+      <c r="B76" s="0">
+        <v>0</v>
+      </c>
+      <c r="C76" s="0">
+        <v>0</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="0">
+        <v>0</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H76" s="0">
+        <v>9788575222942</v>
+      </c>
+      <c r="I76" s="0">
+        <v>128.34</v>
+      </c>
+      <c r="J76" s="0"/>
+      <c r="K76" s="0"/>
+      <c r="L76" s="0"/>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="0">
+        <v>12423</v>
+      </c>
+      <c r="B77" s="0">
+        <v>0</v>
+      </c>
+      <c r="C77" s="0">
+        <v>0</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="0">
+        <v>0</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H77" s="0">
+        <v>9789896685799</v>
+      </c>
+      <c r="I77" s="0">
+        <v>87.42</v>
+      </c>
+      <c r="J77" s="0"/>
+      <c r="K77" s="0"/>
+      <c r="L77" s="0"/>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="0">
+        <v>12424</v>
+      </c>
+      <c r="B78" s="0">
+        <v>0</v>
+      </c>
+      <c r="C78" s="0">
+        <v>0</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="0">
+        <v>0</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H78" s="0">
+        <v>9788582401682</v>
+      </c>
+      <c r="I78" s="0">
+        <v>73.47</v>
+      </c>
+      <c r="J78" s="0"/>
+      <c r="K78" s="0"/>
+      <c r="L78" s="0"/>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="0">
+        <v>12425</v>
+      </c>
+      <c r="B79" s="0">
+        <v>0</v>
+      </c>
+      <c r="C79" s="0">
+        <v>0</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="0">
+        <v>0</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="0">
+        <v>9788522431472</v>
+      </c>
+      <c r="I79" s="0">
+        <v>308.76</v>
+      </c>
+      <c r="J79" s="0"/>
+      <c r="K79" s="0"/>
+      <c r="L79" s="0"/>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="0">
+        <v>12426</v>
+      </c>
+      <c r="B80" s="0">
+        <v>0</v>
+      </c>
+      <c r="C80" s="0">
+        <v>0</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="0">
+        <v>0</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="0">
+        <v>9788539105076</v>
+      </c>
+      <c r="I80" s="0">
+        <v>133.92</v>
+      </c>
+      <c r="J80" s="0"/>
+      <c r="K80" s="0"/>
+      <c r="L80" s="0"/>
+    </row>
+    <row r="81" spans="1:12">
+      <c r="A81" s="0">
+        <v>12427</v>
+      </c>
+      <c r="B81" s="0">
+        <v>0</v>
+      </c>
+      <c r="C81" s="0">
+        <v>0</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="0">
+        <v>0</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H81" s="0">
+        <v>9788537010532</v>
+      </c>
+      <c r="I81" s="0">
+        <v>93</v>
+      </c>
+      <c r="J81" s="0"/>
+      <c r="K81" s="0"/>
+      <c r="L81" s="0"/>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="A82" s="0">
+        <v>12428</v>
+      </c>
+      <c r="B82" s="0">
+        <v>0</v>
+      </c>
+      <c r="C82" s="0">
+        <v>1</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="0">
+        <v>0</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" s="0">
+        <v>9788525054166</v>
+      </c>
+      <c r="I82" s="0">
+        <v>86.49</v>
+      </c>
+      <c r="J82" s="0"/>
+      <c r="K82" s="0"/>
+      <c r="L82" s="0"/>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="A83" s="0">
+        <v>12429</v>
+      </c>
+      <c r="B83" s="0">
+        <v>0</v>
+      </c>
+      <c r="C83" s="0">
+        <v>1</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="0">
+        <v>0</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H83" s="0">
+        <v>9788539002726</v>
+      </c>
+      <c r="I83" s="0">
+        <v>38.13</v>
+      </c>
+      <c r="J83" s="0"/>
+      <c r="K83" s="0"/>
+      <c r="L83" s="0"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
feat: usuário notificado sobre sucesso do envio de arquivo
</commit_message>
<xml_diff>
--- a/public/pdocrud/downloads/file.xlsx
+++ b/public/pdocrud/downloads/file.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>Nº</t>
   </si>
@@ -56,271 +56,226 @@
     <t>BR</t>
   </si>
   <si>
-    <t>701-1209192-6307443</t>
-  </si>
-  <si>
-    <t>2022-10-17</t>
-  </si>
-  <si>
-    <t>701-5391599-9583442</t>
-  </si>
-  <si>
-    <t>701-9461494-3193865</t>
-  </si>
-  <si>
-    <t>2022-10-10</t>
-  </si>
-  <si>
-    <t>701-1423875-1510639</t>
-  </si>
-  <si>
-    <t>701-7893180-7415467</t>
-  </si>
-  <si>
-    <t>701-4662593-4197832</t>
-  </si>
-  <si>
-    <t>701-5775264-6934636</t>
-  </si>
-  <si>
-    <t>702-5526068-5962645</t>
-  </si>
-  <si>
-    <t>701-7493483-1423456</t>
-  </si>
-  <si>
-    <t>701-5293915-9535416</t>
-  </si>
-  <si>
-    <t>702-2963167-6366631</t>
-  </si>
-  <si>
-    <t>702-4090557-3105812</t>
-  </si>
-  <si>
-    <t>701-3223676-8859424</t>
-  </si>
-  <si>
-    <t>702-3127098-8826647</t>
-  </si>
-  <si>
-    <t>702-2653338-7662652</t>
-  </si>
-  <si>
-    <t>702-6459266-5049036</t>
+    <t>702-0301126-6962653</t>
+  </si>
+  <si>
+    <t>2022-10-11</t>
+  </si>
+  <si>
+    <t>702-4676011-9893811</t>
+  </si>
+  <si>
+    <t>702-6555950-5757803</t>
+  </si>
+  <si>
+    <t>2022-10-18</t>
+  </si>
+  <si>
+    <t>702-5440402-8721839</t>
+  </si>
+  <si>
+    <t>701-7191256-8236219</t>
+  </si>
+  <si>
+    <t>701-0241463-6156255</t>
+  </si>
+  <si>
+    <t>702-9480335-8317040</t>
+  </si>
+  <si>
+    <t>702-1901260-2448222</t>
+  </si>
+  <si>
+    <t>702-8018276-0050645</t>
+  </si>
+  <si>
+    <t>701-8538396-7452263</t>
+  </si>
+  <si>
+    <t>701-3652532-5531441</t>
+  </si>
+  <si>
+    <t>701-3095127-8325027</t>
+  </si>
+  <si>
+    <t>702-2121390-7642609</t>
+  </si>
+  <si>
+    <t>702-6286804-1874663</t>
+  </si>
+  <si>
+    <t>701-5656276-9374607</t>
+  </si>
+  <si>
+    <t>701-6096070-9120248</t>
+  </si>
+  <si>
+    <t>702-3552036-2733065</t>
   </si>
   <si>
     <t>US</t>
   </si>
   <si>
-    <t>113-8137802-5444221</t>
-  </si>
-  <si>
-    <t>2022-11-07</t>
-  </si>
-  <si>
-    <t>701-2605761-1778604</t>
-  </si>
-  <si>
-    <t>702-4734067-9853868</t>
-  </si>
-  <si>
-    <t>701-4675306-2159426</t>
-  </si>
-  <si>
-    <t>702-8581848-5065867</t>
-  </si>
-  <si>
-    <t>701-1081896-4552200</t>
-  </si>
-  <si>
-    <t>701-0398557-7225030</t>
-  </si>
-  <si>
-    <t>702-6412282-6492252</t>
-  </si>
-  <si>
-    <t>701-9441835-8365027</t>
-  </si>
-  <si>
-    <t>702-0541042-7986612</t>
-  </si>
-  <si>
-    <t>701-2774317-8808253</t>
-  </si>
-  <si>
-    <t>701-6714138-2493032</t>
-  </si>
-  <si>
-    <t>701-5820993-4525858</t>
-  </si>
-  <si>
-    <t>702-1371093-4160222</t>
-  </si>
-  <si>
-    <t>702-6429587-6356255</t>
-  </si>
-  <si>
-    <t>702-3154588-7526647</t>
-  </si>
-  <si>
-    <t>701-1935748-4582646</t>
-  </si>
-  <si>
-    <t>702-6244304-2801803</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>701-1580357-9105839</t>
+    <t>113-9690156-4182662</t>
+  </si>
+  <si>
+    <t>2022-10-12</t>
+  </si>
+  <si>
+    <t>701-4386995-3840217</t>
+  </si>
+  <si>
+    <t>702-2048692-0679466</t>
+  </si>
+  <si>
+    <t>702-3062767-3560260</t>
+  </si>
+  <si>
+    <t>701-5586890-0711409</t>
+  </si>
+  <si>
+    <t>701-1961755-1912253</t>
+  </si>
+  <si>
+    <t>701-8031148-0687439</t>
+  </si>
+  <si>
+    <t>702-2133711-8725016</t>
+  </si>
+  <si>
+    <t>702-5676721-3163459</t>
+  </si>
+  <si>
+    <t>702-1055762-6005004</t>
+  </si>
+  <si>
+    <t>701-8477567-2120265</t>
+  </si>
+  <si>
+    <t>112-5119624-0537036</t>
+  </si>
+  <si>
+    <t>702-2726097-5554639</t>
+  </si>
+  <si>
+    <t>701-1897862-3369832</t>
+  </si>
+  <si>
+    <t>701-2992681-3951413</t>
+  </si>
+  <si>
+    <t>701-6421891-0055467</t>
+  </si>
+  <si>
+    <t>701-1656330-8104252</t>
+  </si>
+  <si>
+    <t>701-1014460-5794610</t>
+  </si>
+  <si>
+    <t>702-2716206-6199465</t>
+  </si>
+  <si>
+    <t>701-8394361-8625067</t>
+  </si>
+  <si>
+    <t>701-8054307-6751450</t>
+  </si>
+  <si>
+    <t>701-2258676-4696224</t>
+  </si>
+  <si>
+    <t>702-6549096-5560255</t>
+  </si>
+  <si>
+    <t>701-0535754-5488269</t>
+  </si>
+  <si>
+    <t>702-2977962-2073030</t>
+  </si>
+  <si>
+    <t>702-7583732-9441857</t>
+  </si>
+  <si>
+    <t>702-1343361-2017853</t>
+  </si>
+  <si>
+    <t>112-9158632-5907456</t>
   </si>
   <si>
     <t>2022-11-08</t>
   </si>
   <si>
-    <t>702-4319804-1909063</t>
-  </si>
-  <si>
-    <t>701-6180967-0748219</t>
-  </si>
-  <si>
-    <t>702-2860534-4951409</t>
-  </si>
-  <si>
-    <t>701-1056413-0229820</t>
-  </si>
-  <si>
-    <t>701-6369273-9421046</t>
-  </si>
-  <si>
-    <t>701-9976800-4362654</t>
-  </si>
-  <si>
-    <t>702-5084301-3141067</t>
-  </si>
-  <si>
-    <t>702-1007666-4930622</t>
-  </si>
-  <si>
-    <t>702-7303982-1342657</t>
-  </si>
-  <si>
-    <t>701-7187841-0541022</t>
-  </si>
-  <si>
-    <t>702-1956965-6965062</t>
-  </si>
-  <si>
-    <t>702-5960361-3817816</t>
-  </si>
-  <si>
-    <t>701-6560153-4031461</t>
-  </si>
-  <si>
-    <t>701-5283875-4744257</t>
-  </si>
-  <si>
-    <t>701-7000366-9801049</t>
-  </si>
-  <si>
-    <t>702-1474427-3393039</t>
-  </si>
-  <si>
-    <t>702-3494985-0964218</t>
-  </si>
-  <si>
-    <t>701-4376754-9769800</t>
-  </si>
-  <si>
-    <t>702-3331615-1770624</t>
-  </si>
-  <si>
-    <t>702-8864712-0677844</t>
-  </si>
-  <si>
-    <t>702-7945653-1627415</t>
-  </si>
-  <si>
-    <t>702-2176046-8541054</t>
-  </si>
-  <si>
-    <t>702-3620970-5012201</t>
-  </si>
-  <si>
-    <t>701-0592148-9426661</t>
-  </si>
-  <si>
-    <t>702-9244063-0976253</t>
-  </si>
-  <si>
-    <t>702-2058268-2175411</t>
-  </si>
-  <si>
-    <t>702-6654138-6794611</t>
-  </si>
-  <si>
-    <t>701-0140848-0867453</t>
-  </si>
-  <si>
-    <t>702-7673869-9285807</t>
-  </si>
-  <si>
-    <t>701-7600192-1835446</t>
-  </si>
-  <si>
-    <t>701-5120795-3460251</t>
-  </si>
-  <si>
-    <t>702-3824538-1708264</t>
-  </si>
-  <si>
-    <t>702-5431481-8183461</t>
-  </si>
-  <si>
-    <t>701-7154317-1124224</t>
-  </si>
-  <si>
-    <t>701-9008725-3339420</t>
-  </si>
-  <si>
-    <t>701-2313265-9166657</t>
-  </si>
-  <si>
-    <t>702-4367131-3214669</t>
-  </si>
-  <si>
-    <t>702-2154948-3252256</t>
-  </si>
-  <si>
-    <t>702-5526123-5562660</t>
-  </si>
-  <si>
-    <t>702-2672290-7623402</t>
-  </si>
-  <si>
-    <t>702-0551478-1147421</t>
-  </si>
-  <si>
-    <t>702-9588226-6843425</t>
-  </si>
-  <si>
-    <t>702-0522937-4361011</t>
-  </si>
-  <si>
-    <t>701-4446158-9705043</t>
-  </si>
-  <si>
-    <t>702-3448042-2531437</t>
-  </si>
-  <si>
-    <t>2022-10-11</t>
-  </si>
-  <si>
-    <t>701-5400778-0580268</t>
-  </si>
-  <si>
-    <t>702-2711942-9791437</t>
+    <t>701-7356782-5831421</t>
+  </si>
+  <si>
+    <t>701-6587264-5319466</t>
+  </si>
+  <si>
+    <t>702-3858578-7439423</t>
+  </si>
+  <si>
+    <t>702-0462013-9523453</t>
+  </si>
+  <si>
+    <t>702-3541423-4745804</t>
+  </si>
+  <si>
+    <t>701-4961401-3246634</t>
+  </si>
+  <si>
+    <t>2022-10-13</t>
+  </si>
+  <si>
+    <t>701-0011562-9185874</t>
+  </si>
+  <si>
+    <t>112-6531321-2141809</t>
+  </si>
+  <si>
+    <t>2022-10-19</t>
+  </si>
+  <si>
+    <t>702-3101478-4647401</t>
+  </si>
+  <si>
+    <t>701-2479898-6504244</t>
+  </si>
+  <si>
+    <t>702-6323620-8935460</t>
+  </si>
+  <si>
+    <t>702-9448552-8569834</t>
+  </si>
+  <si>
+    <t>701-0871676-1195451</t>
+  </si>
+  <si>
+    <t>702-4189461-3051419</t>
+  </si>
+  <si>
+    <t>702-6652192-6094605</t>
+  </si>
+  <si>
+    <t>701-5821235-1281820</t>
+  </si>
+  <si>
+    <t>701-0055189-8643442</t>
+  </si>
+  <si>
+    <t>701-8930215-8960223</t>
+  </si>
+  <si>
+    <t>701-0007640-9915405</t>
+  </si>
+  <si>
+    <t>701-5217726-3133855</t>
+  </si>
+  <si>
+    <t>2022-10-07</t>
+  </si>
+  <si>
+    <t>702-5301893-2231413</t>
   </si>
 </sst>
 </file>
@@ -659,7 +614,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -707,7 +662,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="0">
-        <v>12348</v>
+        <v>12429</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -728,10 +683,10 @@
         <v>14</v>
       </c>
       <c r="H2" s="0">
-        <v>9788586584022</v>
+        <v>9788574209876</v>
       </c>
       <c r="I2" s="0">
-        <v>79.05</v>
+        <v>85.56</v>
       </c>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
@@ -739,7 +694,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="0">
-        <v>12349</v>
+        <v>12430</v>
       </c>
       <c r="B3" s="0">
         <v>0</v>
@@ -760,10 +715,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="0">
-        <v>9788583000044</v>
+        <v>9788594540607</v>
       </c>
       <c r="I3" s="0">
-        <v>151.59</v>
+        <v>125.55</v>
       </c>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
@@ -771,7 +726,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="0">
-        <v>12350</v>
+        <v>12431</v>
       </c>
       <c r="B4" s="0">
         <v>0</v>
@@ -792,10 +747,10 @@
         <v>17</v>
       </c>
       <c r="H4" s="0">
-        <v>9788580408935</v>
+        <v>9788544238042</v>
       </c>
       <c r="I4" s="0">
-        <v>255.75</v>
+        <v>248.31</v>
       </c>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
@@ -803,7 +758,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="0">
-        <v>12351</v>
+        <v>12432</v>
       </c>
       <c r="B5" s="0">
         <v>0</v>
@@ -821,13 +776,13 @@
         <v>18</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0">
-        <v>9788522470716</v>
+        <v>9789896685799</v>
       </c>
       <c r="I5" s="0">
-        <v>156.24</v>
+        <v>87.42</v>
       </c>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
@@ -835,7 +790,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="0">
-        <v>12352</v>
+        <v>12433</v>
       </c>
       <c r="B6" s="0">
         <v>0</v>
@@ -856,10 +811,10 @@
         <v>14</v>
       </c>
       <c r="H6" s="0">
-        <v>9780857625410</v>
+        <v>9788578540791</v>
       </c>
       <c r="I6" s="0">
-        <v>154.38</v>
+        <v>114.39</v>
       </c>
       <c r="J6" s="0"/>
       <c r="K6" s="0"/>
@@ -867,7 +822,7 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="0">
-        <v>12353</v>
+        <v>12434</v>
       </c>
       <c r="B7" s="0">
         <v>0</v>
@@ -888,10 +843,10 @@
         <v>17</v>
       </c>
       <c r="H7" s="0">
-        <v>9788533604858</v>
+        <v>9788542213300</v>
       </c>
       <c r="I7" s="0">
-        <v>69.75</v>
+        <v>104.16</v>
       </c>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
@@ -899,7 +854,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="0">
-        <v>12354</v>
+        <v>12435</v>
       </c>
       <c r="B8" s="0">
         <v>0</v>
@@ -917,13 +872,13 @@
         <v>21</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H8" s="0">
-        <v>9788582604953</v>
+        <v>9788578540791</v>
       </c>
       <c r="I8" s="0">
-        <v>275.28</v>
+        <v>114.39</v>
       </c>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
@@ -931,7 +886,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="0">
-        <v>12355</v>
+        <v>12436</v>
       </c>
       <c r="B9" s="0">
         <v>0</v>
@@ -946,16 +901,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="0">
-        <v>9788535903454</v>
+        <v>9788585480400</v>
       </c>
       <c r="I9" s="0">
-        <v>57.66</v>
+        <v>105.09</v>
       </c>
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
@@ -963,7 +918,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="0">
-        <v>12356</v>
+        <v>12437</v>
       </c>
       <c r="B10" s="0">
         <v>0</v>
@@ -978,16 +933,16 @@
         <v>0</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H10" s="0">
-        <v>9788516051716</v>
+        <v>9788575030936</v>
       </c>
       <c r="I10" s="0">
-        <v>130.2</v>
+        <v>163.68</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
@@ -995,7 +950,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="0">
-        <v>12357</v>
+        <v>12438</v>
       </c>
       <c r="B11" s="0">
         <v>0</v>
@@ -1010,16 +965,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="0">
-        <v>7895377000677</v>
+        <v>9788521903406</v>
       </c>
       <c r="I11" s="0">
-        <v>232.5</v>
+        <v>107.88</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
@@ -1027,7 +982,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="0">
-        <v>12358</v>
+        <v>12439</v>
       </c>
       <c r="B12" s="0">
         <v>0</v>
@@ -1042,16 +997,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="0">
-        <v>9788534921961</v>
+        <v>9788535907742</v>
       </c>
       <c r="I12" s="0">
-        <v>243.66</v>
+        <v>113.46</v>
       </c>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
@@ -1059,7 +1014,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="0">
-        <v>12359</v>
+        <v>12440</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
@@ -1074,16 +1029,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="0">
-        <v>9788565985260</v>
+        <v>9788543104911</v>
       </c>
       <c r="I13" s="0">
-        <v>163.68</v>
+        <v>88.35</v>
       </c>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
@@ -1091,7 +1046,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="0">
-        <v>12360</v>
+        <v>12441</v>
       </c>
       <c r="B14" s="0">
         <v>0</v>
@@ -1106,16 +1061,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="0">
-        <v>9788530983178</v>
+        <v>9788584257188</v>
       </c>
       <c r="I14" s="0">
-        <v>323.64</v>
+        <v>200.88</v>
       </c>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
@@ -1123,7 +1078,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="0">
-        <v>12361</v>
+        <v>12442</v>
       </c>
       <c r="B15" s="0">
         <v>0</v>
@@ -1138,16 +1093,16 @@
         <v>0</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H15" s="0">
-        <v>9788551804247</v>
+        <v>9788594188908</v>
       </c>
       <c r="I15" s="0">
-        <v>92.07</v>
+        <v>148.8</v>
       </c>
       <c r="J15" s="0"/>
       <c r="K15" s="0"/>
@@ -1155,7 +1110,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="0">
-        <v>12362</v>
+        <v>12443</v>
       </c>
       <c r="B16" s="0">
         <v>0</v>
@@ -1170,16 +1125,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H16" s="0">
-        <v>9788544237793</v>
+        <v>9786586025811</v>
       </c>
       <c r="I16" s="0">
-        <v>446.4</v>
+        <v>165.54</v>
       </c>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
@@ -1187,7 +1142,7 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="0">
-        <v>12363</v>
+        <v>12444</v>
       </c>
       <c r="B17" s="0">
         <v>0</v>
@@ -1202,16 +1157,16 @@
         <v>0</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="0">
-        <v>9788577010585</v>
+        <v>9788560303342</v>
       </c>
       <c r="I17" s="0">
-        <v>130.2</v>
+        <v>73.47</v>
       </c>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -1219,7 +1174,7 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="0">
-        <v>12364</v>
+        <v>12445</v>
       </c>
       <c r="B18" s="0">
         <v>0</v>
@@ -1228,22 +1183,22 @@
         <v>0</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0">
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="H18" s="0">
-        <v>9788580092813</v>
+        <v>9788544107546</v>
       </c>
       <c r="I18" s="0">
-        <v>130.2</v>
+        <v>102.3</v>
       </c>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -1251,7 +1206,7 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="0">
-        <v>12365</v>
+        <v>12446</v>
       </c>
       <c r="B19" s="0">
         <v>0</v>
@@ -1266,16 +1221,16 @@
         <v>0</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H19" s="0">
-        <v>9788535287158</v>
+        <v>9788527725170</v>
       </c>
       <c r="I19" s="0">
-        <v>401.76</v>
+        <v>398.97</v>
       </c>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
@@ -1283,7 +1238,7 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="0">
-        <v>12366</v>
+        <v>12447</v>
       </c>
       <c r="B20" s="0">
         <v>0</v>
@@ -1292,22 +1247,22 @@
         <v>0</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E20" s="0">
         <v>0</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H20" s="0">
-        <v>9788576089742</v>
+        <v>9788531416651</v>
       </c>
       <c r="I20" s="0">
-        <v>140.43</v>
+        <v>61.38</v>
       </c>
       <c r="J20" s="0"/>
       <c r="K20" s="0"/>
@@ -1315,7 +1270,7 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="0">
-        <v>12367</v>
+        <v>12448</v>
       </c>
       <c r="B21" s="0">
         <v>0</v>
@@ -1330,16 +1285,16 @@
         <v>0</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H21" s="0">
-        <v>9788583100195</v>
+        <v>9789898855732</v>
       </c>
       <c r="I21" s="0">
-        <v>269.7</v>
+        <v>122.76</v>
       </c>
       <c r="J21" s="0"/>
       <c r="K21" s="0"/>
@@ -1347,7 +1302,7 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="0">
-        <v>12368</v>
+        <v>12449</v>
       </c>
       <c r="B22" s="0">
         <v>0</v>
@@ -1362,16 +1317,16 @@
         <v>0</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H22" s="0">
-        <v>9788581301570</v>
+        <v>9788501070791</v>
       </c>
       <c r="I22" s="0">
-        <v>111.6</v>
+        <v>79.05</v>
       </c>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
@@ -1379,7 +1334,7 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="0">
-        <v>12369</v>
+        <v>12450</v>
       </c>
       <c r="B23" s="0">
         <v>0</v>
@@ -1394,16 +1349,16 @@
         <v>0</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="0">
-        <v>9786586093377</v>
+        <v>9788539506637</v>
       </c>
       <c r="I23" s="0">
-        <v>141.36</v>
+        <v>167.4</v>
       </c>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
@@ -1411,7 +1366,7 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="0">
-        <v>12370</v>
+        <v>12451</v>
       </c>
       <c r="B24" s="0">
         <v>0</v>
@@ -1426,16 +1381,16 @@
         <v>0</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H24" s="0">
-        <v>9788578542061</v>
+        <v>9788542213300</v>
       </c>
       <c r="I24" s="0">
-        <v>122.76</v>
+        <v>104.16</v>
       </c>
       <c r="J24" s="0"/>
       <c r="K24" s="0"/>
@@ -1443,7 +1398,7 @@
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="0">
-        <v>12371</v>
+        <v>12452</v>
       </c>
       <c r="B25" s="0">
         <v>0</v>
@@ -1458,16 +1413,16 @@
         <v>0</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H25" s="0">
-        <v>9788502636293</v>
+        <v>9786555110005</v>
       </c>
       <c r="I25" s="0">
-        <v>146.94</v>
+        <v>76.26</v>
       </c>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
@@ -1475,7 +1430,7 @@
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="0">
-        <v>12372</v>
+        <v>12453</v>
       </c>
       <c r="B26" s="0">
         <v>0</v>
@@ -1490,16 +1445,16 @@
         <v>0</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H26" s="0">
-        <v>9788531611292</v>
+        <v>9788573124835</v>
       </c>
       <c r="I26" s="0">
-        <v>102.3</v>
+        <v>116.25</v>
       </c>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
@@ -1507,7 +1462,7 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="0">
-        <v>12373</v>
+        <v>12454</v>
       </c>
       <c r="B27" s="0">
         <v>0</v>
@@ -1522,16 +1477,16 @@
         <v>0</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="0">
-        <v>9788545006046</v>
+        <v>9788571106123</v>
       </c>
       <c r="I27" s="0">
-        <v>226.92</v>
+        <v>74.4</v>
       </c>
       <c r="J27" s="0"/>
       <c r="K27" s="0"/>
@@ -1539,7 +1494,7 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="0">
-        <v>12374</v>
+        <v>12455</v>
       </c>
       <c r="B28" s="0">
         <v>0</v>
@@ -1554,16 +1509,16 @@
         <v>0</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="0">
-        <v>9788535919714</v>
+        <v>9788582401903</v>
       </c>
       <c r="I28" s="0">
-        <v>88.35</v>
+        <v>92.07</v>
       </c>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
@@ -1571,7 +1526,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="0">
-        <v>12375</v>
+        <v>12456</v>
       </c>
       <c r="B29" s="0">
         <v>0</v>
@@ -1586,16 +1541,16 @@
         <v>0</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H29" s="0">
-        <v>9788577893515</v>
+        <v>9788530980566</v>
       </c>
       <c r="I29" s="0">
-        <v>171.12</v>
+        <v>725.4</v>
       </c>
       <c r="J29" s="0"/>
       <c r="K29" s="0"/>
@@ -1603,7 +1558,7 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="0">
-        <v>12376</v>
+        <v>12457</v>
       </c>
       <c r="B30" s="0">
         <v>0</v>
@@ -1618,16 +1573,16 @@
         <v>0</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H30" s="0">
-        <v>9788561467166</v>
+        <v>9788574960340</v>
       </c>
       <c r="I30" s="0">
-        <v>93.93</v>
+        <v>67.89</v>
       </c>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
@@ -1635,7 +1590,7 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="0">
-        <v>12377</v>
+        <v>12458</v>
       </c>
       <c r="B31" s="0">
         <v>0</v>
@@ -1644,22 +1599,22 @@
         <v>0</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E31" s="0">
         <v>0</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="H31" s="0">
-        <v>9788578542238</v>
+        <v>9788535245172</v>
       </c>
       <c r="I31" s="0">
-        <v>133.92</v>
+        <v>46.5</v>
       </c>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
@@ -1667,7 +1622,7 @@
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="0">
-        <v>12378</v>
+        <v>12459</v>
       </c>
       <c r="B32" s="0">
         <v>0</v>
@@ -1682,16 +1637,16 @@
         <v>0</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H32" s="0">
-        <v>9788554085018</v>
+        <v>9788556270092</v>
       </c>
       <c r="I32" s="0">
-        <v>353.4</v>
+        <v>71.61</v>
       </c>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
@@ -1699,7 +1654,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="0">
-        <v>12379</v>
+        <v>12460</v>
       </c>
       <c r="B33" s="0">
         <v>0</v>
@@ -1714,16 +1669,16 @@
         <v>0</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G33" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="0">
-        <v>9788578230753</v>
+        <v>9788556270108</v>
       </c>
       <c r="I33" s="0">
-        <v>96.72</v>
+        <v>79.98</v>
       </c>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
@@ -1731,7 +1686,7 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="0">
-        <v>12380</v>
+        <v>12461</v>
       </c>
       <c r="B34" s="0">
         <v>0</v>
@@ -1746,16 +1701,16 @@
         <v>0</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G34" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H34" s="0">
-        <v>9788594540416</v>
+        <v>9789895612062</v>
       </c>
       <c r="I34" s="0">
-        <v>130.2</v>
+        <v>74.4</v>
       </c>
       <c r="J34" s="0"/>
       <c r="K34" s="0"/>
@@ -1763,7 +1718,7 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="0">
-        <v>12381</v>
+        <v>12462</v>
       </c>
       <c r="B35" s="0">
         <v>0</v>
@@ -1778,16 +1733,16 @@
         <v>0</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G35" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="0">
-        <v>9788575033890</v>
+        <v>9788502211742</v>
       </c>
       <c r="I35" s="0">
-        <v>75.33</v>
+        <v>241.8</v>
       </c>
       <c r="J35" s="0"/>
       <c r="K35" s="0"/>
@@ -1795,7 +1750,7 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="0">
-        <v>12382</v>
+        <v>12463</v>
       </c>
       <c r="B36" s="0">
         <v>0</v>
@@ -1804,22 +1759,22 @@
         <v>0</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="E36" s="0">
         <v>0</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="H36" s="0">
-        <v>9788547310288</v>
+        <v>9788545712367</v>
       </c>
       <c r="I36" s="0">
-        <v>56</v>
+        <v>154.38</v>
       </c>
       <c r="J36" s="0"/>
       <c r="K36" s="0"/>
@@ -1827,7 +1782,7 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="0">
-        <v>12383</v>
+        <v>12464</v>
       </c>
       <c r="B37" s="0">
         <v>0</v>
@@ -1842,16 +1797,16 @@
         <v>0</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G37" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H37" s="0">
-        <v>9788503011082</v>
+        <v>9788535909616</v>
       </c>
       <c r="I37" s="0">
-        <v>130.2</v>
+        <v>120.9</v>
       </c>
       <c r="J37" s="0"/>
       <c r="K37" s="0"/>
@@ -1859,7 +1814,7 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="0">
-        <v>12384</v>
+        <v>12465</v>
       </c>
       <c r="B38" s="0">
         <v>0</v>
@@ -1874,16 +1829,16 @@
         <v>0</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H38" s="0">
-        <v>9788538810292</v>
+        <v>9788535912678</v>
       </c>
       <c r="I38" s="0">
-        <v>265.98</v>
+        <v>113.46</v>
       </c>
       <c r="J38" s="0"/>
       <c r="K38" s="0"/>
@@ -1891,7 +1846,7 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="0">
-        <v>12385</v>
+        <v>12466</v>
       </c>
       <c r="B39" s="0">
         <v>0</v>
@@ -1906,16 +1861,16 @@
         <v>0</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H39" s="0">
-        <v>9788520942215</v>
+        <v>9786589760450</v>
       </c>
       <c r="I39" s="0">
-        <v>334.8</v>
+        <v>109.74</v>
       </c>
       <c r="J39" s="0"/>
       <c r="K39" s="0"/>
@@ -1923,7 +1878,7 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="0">
-        <v>12386</v>
+        <v>12467</v>
       </c>
       <c r="B40" s="0">
         <v>0</v>
@@ -1938,16 +1893,16 @@
         <v>0</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H40" s="0">
-        <v>9788535909432</v>
+        <v>9788569214212</v>
       </c>
       <c r="I40" s="0">
-        <v>74.4</v>
+        <v>162.75</v>
       </c>
       <c r="J40" s="0"/>
       <c r="K40" s="0"/>
@@ -1955,7 +1910,7 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="0">
-        <v>12387</v>
+        <v>12468</v>
       </c>
       <c r="B41" s="0">
         <v>0</v>
@@ -1970,16 +1925,16 @@
         <v>0</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G41" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H41" s="0">
-        <v>9788573255515</v>
+        <v>9788502083899</v>
       </c>
       <c r="I41" s="0">
-        <v>70.68</v>
+        <v>195.3</v>
       </c>
       <c r="J41" s="0"/>
       <c r="K41" s="0"/>
@@ -1987,7 +1942,7 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="0">
-        <v>12388</v>
+        <v>12469</v>
       </c>
       <c r="B42" s="0">
         <v>0</v>
@@ -2002,16 +1957,16 @@
         <v>0</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G42" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H42" s="0">
-        <v>9788576170464</v>
+        <v>9788564468771</v>
       </c>
       <c r="I42" s="0">
-        <v>66.96</v>
+        <v>107.88</v>
       </c>
       <c r="J42" s="0"/>
       <c r="K42" s="0"/>
@@ -2019,7 +1974,7 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="0">
-        <v>12389</v>
+        <v>12470</v>
       </c>
       <c r="B43" s="0">
         <v>0</v>
@@ -2034,16 +1989,16 @@
         <v>0</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H43" s="0">
-        <v>9788577852673</v>
+        <v>9788522496082</v>
       </c>
       <c r="I43" s="0">
-        <v>88.35</v>
+        <v>243.66</v>
       </c>
       <c r="J43" s="0"/>
       <c r="K43" s="0"/>
@@ -2051,7 +2006,7 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="0">
-        <v>12390</v>
+        <v>12471</v>
       </c>
       <c r="B44" s="0">
         <v>0</v>
@@ -2066,16 +2021,16 @@
         <v>0</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G44" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H44" s="0">
-        <v>9788535919714</v>
+        <v>9788525052407</v>
       </c>
       <c r="I44" s="0">
-        <v>88.35</v>
+        <v>121.83</v>
       </c>
       <c r="J44" s="0"/>
       <c r="K44" s="0"/>
@@ -2083,7 +2038,7 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="0">
-        <v>12391</v>
+        <v>12472</v>
       </c>
       <c r="B45" s="0">
         <v>0</v>
@@ -2098,16 +2053,16 @@
         <v>0</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H45" s="0">
-        <v>9788527727631</v>
+        <v>9788536124247</v>
       </c>
       <c r="I45" s="0">
-        <v>671.46</v>
+        <v>251.1</v>
       </c>
       <c r="J45" s="0"/>
       <c r="K45" s="0"/>
@@ -2115,7 +2070,7 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="0">
-        <v>12392</v>
+        <v>12473</v>
       </c>
       <c r="B46" s="0">
         <v>0</v>
@@ -2130,16 +2085,16 @@
         <v>0</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H46" s="0">
-        <v>9788582424056</v>
+        <v>9788577004232</v>
       </c>
       <c r="I46" s="0">
-        <v>221.34</v>
+        <v>249.24</v>
       </c>
       <c r="J46" s="0"/>
       <c r="K46" s="0"/>
@@ -2147,7 +2102,7 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="0">
-        <v>12393</v>
+        <v>12474</v>
       </c>
       <c r="B47" s="0">
         <v>0</v>
@@ -2162,16 +2117,16 @@
         <v>0</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G47" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H47" s="0">
-        <v>9788581744209</v>
+        <v>9788538074427</v>
       </c>
       <c r="I47" s="0">
-        <v>254.82</v>
+        <v>82.77</v>
       </c>
       <c r="J47" s="0"/>
       <c r="K47" s="0"/>
@@ -2179,7 +2134,7 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="0">
-        <v>12394</v>
+        <v>12475</v>
       </c>
       <c r="B48" s="0">
         <v>0</v>
@@ -2194,16 +2149,16 @@
         <v>0</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G48" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H48" s="0">
-        <v>9788595010154</v>
+        <v>9788581488400</v>
       </c>
       <c r="I48" s="0">
-        <v>252.96</v>
+        <v>103.23</v>
       </c>
       <c r="J48" s="0"/>
       <c r="K48" s="0"/>
@@ -2211,7 +2166,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="0">
-        <v>12395</v>
+        <v>12476</v>
       </c>
       <c r="B49" s="0">
         <v>0</v>
@@ -2220,22 +2175,22 @@
         <v>0</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E49" s="0">
         <v>0</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="H49" s="0">
-        <v>9788576651703</v>
+        <v>9788534521185</v>
       </c>
       <c r="I49" s="0">
-        <v>74.4</v>
+        <v>37.2</v>
       </c>
       <c r="J49" s="0"/>
       <c r="K49" s="0"/>
@@ -2243,7 +2198,7 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="0">
-        <v>12396</v>
+        <v>12477</v>
       </c>
       <c r="B50" s="0">
         <v>0</v>
@@ -2258,16 +2213,16 @@
         <v>0</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>14</v>
       </c>
       <c r="H50" s="0">
-        <v>9788531406119</v>
+        <v>9786555140101</v>
       </c>
       <c r="I50" s="0">
-        <v>156.24</v>
+        <v>139.5</v>
       </c>
       <c r="J50" s="0"/>
       <c r="K50" s="0"/>
@@ -2275,7 +2230,7 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="0">
-        <v>12397</v>
+        <v>12478</v>
       </c>
       <c r="B51" s="0">
         <v>0</v>
@@ -2290,16 +2245,16 @@
         <v>0</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H51" s="0">
-        <v>9788579144189</v>
+        <v>9788568071052</v>
       </c>
       <c r="I51" s="0">
-        <v>102.3</v>
+        <v>105.09</v>
       </c>
       <c r="J51" s="0"/>
       <c r="K51" s="0"/>
@@ -2307,7 +2262,7 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="0">
-        <v>12398</v>
+        <v>12479</v>
       </c>
       <c r="B52" s="0">
         <v>0</v>
@@ -2322,16 +2277,16 @@
         <v>0</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H52" s="0">
-        <v>9788587199096</v>
+        <v>9788542206081</v>
       </c>
       <c r="I52" s="0">
-        <v>79.05</v>
+        <v>93</v>
       </c>
       <c r="J52" s="0"/>
       <c r="K52" s="0"/>
@@ -2339,7 +2294,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="0">
-        <v>12399</v>
+        <v>12480</v>
       </c>
       <c r="B53" s="0">
         <v>0</v>
@@ -2354,16 +2309,16 @@
         <v>0</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H53" s="0">
-        <v>9788538802846</v>
+        <v>9788535918991</v>
       </c>
       <c r="I53" s="0">
-        <v>583.11</v>
+        <v>183.21</v>
       </c>
       <c r="J53" s="0"/>
       <c r="K53" s="0"/>
@@ -2371,7 +2326,7 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="0">
-        <v>12400</v>
+        <v>12481</v>
       </c>
       <c r="B54" s="0">
         <v>0</v>
@@ -2386,16 +2341,16 @@
         <v>0</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H54" s="0">
-        <v>9786556059914</v>
+        <v>9788520941799</v>
       </c>
       <c r="I54" s="0">
-        <v>170.19</v>
+        <v>111.6</v>
       </c>
       <c r="J54" s="0"/>
       <c r="K54" s="0"/>
@@ -2403,7 +2358,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="0">
-        <v>12401</v>
+        <v>12482</v>
       </c>
       <c r="B55" s="0">
         <v>0</v>
@@ -2418,16 +2373,16 @@
         <v>0</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="H55" s="0">
-        <v>9788575326169</v>
+        <v>9788575421864</v>
       </c>
       <c r="I55" s="0">
-        <v>140.43</v>
+        <v>79.05</v>
       </c>
       <c r="J55" s="0"/>
       <c r="K55" s="0"/>
@@ -2435,7 +2390,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="0">
-        <v>12402</v>
+        <v>12483</v>
       </c>
       <c r="B56" s="0">
         <v>0</v>
@@ -2450,16 +2405,16 @@
         <v>0</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="H56" s="0">
-        <v>9788581496771</v>
+        <v>9788538803898</v>
       </c>
       <c r="I56" s="0">
-        <v>134.85</v>
+        <v>254.82</v>
       </c>
       <c r="J56" s="0"/>
       <c r="K56" s="0"/>
@@ -2467,7 +2422,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="0">
-        <v>12403</v>
+        <v>12484</v>
       </c>
       <c r="B57" s="0">
         <v>0</v>
@@ -2476,22 +2431,22 @@
         <v>0</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E57" s="0">
         <v>0</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H57" s="0">
-        <v>9788567861289</v>
+        <v>9788515035557</v>
       </c>
       <c r="I57" s="0">
-        <v>152.52</v>
+        <v>53.01</v>
       </c>
       <c r="J57" s="0"/>
       <c r="K57" s="0"/>
@@ -2499,7 +2454,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="0">
-        <v>12404</v>
+        <v>12485</v>
       </c>
       <c r="B58" s="0">
         <v>0</v>
@@ -2514,16 +2469,16 @@
         <v>0</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="H58" s="0">
-        <v>9788532510136</v>
+        <v>9788528606744</v>
       </c>
       <c r="I58" s="0">
-        <v>110.67</v>
+        <v>223.2</v>
       </c>
       <c r="J58" s="0"/>
       <c r="K58" s="0"/>
@@ -2531,7 +2486,7 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="0">
-        <v>12405</v>
+        <v>12486</v>
       </c>
       <c r="B59" s="0">
         <v>0</v>
@@ -2546,16 +2501,16 @@
         <v>0</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="H59" s="0">
-        <v>9788532528575</v>
+        <v>9788542206869</v>
       </c>
       <c r="I59" s="0">
-        <v>88.35</v>
+        <v>152.52</v>
       </c>
       <c r="J59" s="0"/>
       <c r="K59" s="0"/>
@@ -2563,7 +2518,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="0">
-        <v>12406</v>
+        <v>12487</v>
       </c>
       <c r="B60" s="0">
         <v>0</v>
@@ -2578,16 +2533,16 @@
         <v>0</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H60" s="0">
-        <v>9788569538042</v>
+        <v>9788531504730</v>
       </c>
       <c r="I60" s="0">
-        <v>135.78</v>
+        <v>105.09</v>
       </c>
       <c r="J60" s="0"/>
       <c r="K60" s="0"/>
@@ -2595,7 +2550,7 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="0">
-        <v>12407</v>
+        <v>12488</v>
       </c>
       <c r="B61" s="0">
         <v>0</v>
@@ -2610,16 +2565,16 @@
         <v>0</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H61" s="0">
-        <v>9788535911282</v>
+        <v>9788530981174</v>
       </c>
       <c r="I61" s="0">
-        <v>213.9</v>
+        <v>254.82</v>
       </c>
       <c r="J61" s="0"/>
       <c r="K61" s="0"/>
@@ -2627,7 +2582,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="0">
-        <v>12408</v>
+        <v>12489</v>
       </c>
       <c r="B62" s="0">
         <v>0</v>
@@ -2642,16 +2597,16 @@
         <v>0</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="H62" s="0">
-        <v>9789723016734</v>
+        <v>9788530960902</v>
       </c>
       <c r="I62" s="0">
-        <v>123.69</v>
+        <v>338.52</v>
       </c>
       <c r="J62" s="0"/>
       <c r="K62" s="0"/>
@@ -2659,7 +2614,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="0">
-        <v>12409</v>
+        <v>12490</v>
       </c>
       <c r="B63" s="0">
         <v>0</v>
@@ -2674,16 +2629,16 @@
         <v>0</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H63" s="0">
-        <v>9788539608683</v>
+        <v>9788525418265</v>
       </c>
       <c r="I63" s="0">
-        <v>132.99</v>
+        <v>93</v>
       </c>
       <c r="J63" s="0"/>
       <c r="K63" s="0"/>
@@ -2691,7 +2646,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="0">
-        <v>12410</v>
+        <v>12491</v>
       </c>
       <c r="B64" s="0">
         <v>0</v>
@@ -2706,16 +2661,16 @@
         <v>0</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="H64" s="0">
-        <v>9788580632040</v>
+        <v>9788599296226</v>
       </c>
       <c r="I64" s="0">
-        <v>73.47</v>
+        <v>74.4</v>
       </c>
       <c r="J64" s="0"/>
       <c r="K64" s="0"/>
@@ -2723,7 +2678,7 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="0">
-        <v>12411</v>
+        <v>12492</v>
       </c>
       <c r="B65" s="0">
         <v>0</v>
@@ -2738,16 +2693,16 @@
         <v>0</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="H65" s="0">
-        <v>9788522450572</v>
+        <v>9788501110619</v>
       </c>
       <c r="I65" s="0">
-        <v>306.9</v>
+        <v>244.59</v>
       </c>
       <c r="J65" s="0"/>
       <c r="K65" s="0"/>
@@ -2755,7 +2710,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="0">
-        <v>12412</v>
+        <v>12493</v>
       </c>
       <c r="B66" s="0">
         <v>0</v>
@@ -2770,16 +2725,16 @@
         <v>0</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="H66" s="0">
-        <v>9788577001200</v>
+        <v>9788599296226</v>
       </c>
       <c r="I66" s="0">
-        <v>165.54</v>
+        <v>74.4</v>
       </c>
       <c r="J66" s="0"/>
       <c r="K66" s="0"/>
@@ -2787,13 +2742,13 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="0">
-        <v>12413</v>
+        <v>12494</v>
       </c>
       <c r="B67" s="0">
         <v>0</v>
       </c>
       <c r="C67" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>12</v>
@@ -2802,16 +2757,16 @@
         <v>0</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="H67" s="0">
-        <v>9788574124032</v>
+        <v>9788526213982</v>
       </c>
       <c r="I67" s="0">
-        <v>95.79</v>
+        <v>118.11</v>
       </c>
       <c r="J67" s="0"/>
       <c r="K67" s="0"/>
@@ -2819,13 +2774,13 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="0">
-        <v>12414</v>
+        <v>12495</v>
       </c>
       <c r="B68" s="0">
         <v>0</v>
       </c>
       <c r="C68" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>12</v>
@@ -2834,16 +2789,16 @@
         <v>0</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="H68" s="0">
-        <v>7898572200972</v>
+        <v>9788580555967</v>
       </c>
       <c r="I68" s="0">
-        <v>244.59</v>
+        <v>889.08</v>
       </c>
       <c r="J68" s="0"/>
       <c r="K68" s="0"/>
@@ -2851,13 +2806,13 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="0">
-        <v>12415</v>
+        <v>12496</v>
       </c>
       <c r="B69" s="0">
         <v>0</v>
       </c>
       <c r="C69" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>12</v>
@@ -2866,16 +2821,16 @@
         <v>0</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="H69" s="0">
-        <v>9788594660619</v>
+        <v>9788589239868</v>
       </c>
       <c r="I69" s="0">
-        <v>96.72</v>
+        <v>47.43</v>
       </c>
       <c r="J69" s="0"/>
       <c r="K69" s="0"/>
@@ -2883,13 +2838,13 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="0">
-        <v>12416</v>
+        <v>12497</v>
       </c>
       <c r="B70" s="0">
         <v>0</v>
       </c>
       <c r="C70" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>12</v>
@@ -2898,436 +2853,20 @@
         <v>0</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H70" s="0">
-        <v>9788537010532</v>
+        <v>9788578812881</v>
       </c>
       <c r="I70" s="0">
-        <v>93</v>
+        <v>38.13</v>
       </c>
       <c r="J70" s="0"/>
       <c r="K70" s="0"/>
       <c r="L70" s="0"/>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="A71" s="0">
-        <v>12417</v>
-      </c>
-      <c r="B71" s="0">
-        <v>0</v>
-      </c>
-      <c r="C71" s="0">
-        <v>0</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" s="0">
-        <v>0</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H71" s="0">
-        <v>9788504020311</v>
-      </c>
-      <c r="I71" s="0">
-        <v>98.58</v>
-      </c>
-      <c r="J71" s="0"/>
-      <c r="K71" s="0"/>
-      <c r="L71" s="0"/>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="A72" s="0">
-        <v>12418</v>
-      </c>
-      <c r="B72" s="0">
-        <v>0</v>
-      </c>
-      <c r="C72" s="0">
-        <v>0</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" s="0">
-        <v>0</v>
-      </c>
-      <c r="F72" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G72" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H72" s="0">
-        <v>9788535247633</v>
-      </c>
-      <c r="I72" s="0">
-        <v>176.7</v>
-      </c>
-      <c r="J72" s="0"/>
-      <c r="K72" s="0"/>
-      <c r="L72" s="0"/>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="A73" s="0">
-        <v>12419</v>
-      </c>
-      <c r="B73" s="0">
-        <v>0</v>
-      </c>
-      <c r="C73" s="0">
-        <v>0</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73" s="0">
-        <v>0</v>
-      </c>
-      <c r="F73" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G73" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H73" s="0">
-        <v>9788562219146</v>
-      </c>
-      <c r="I73" s="0">
-        <v>82.77</v>
-      </c>
-      <c r="J73" s="0"/>
-      <c r="K73" s="0"/>
-      <c r="L73" s="0"/>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="A74" s="0">
-        <v>12420</v>
-      </c>
-      <c r="B74" s="0">
-        <v>0</v>
-      </c>
-      <c r="C74" s="0">
-        <v>0</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" s="0">
-        <v>0</v>
-      </c>
-      <c r="F74" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G74" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H74" s="0">
-        <v>9786558693567</v>
-      </c>
-      <c r="I74" s="0">
-        <v>88.35</v>
-      </c>
-      <c r="J74" s="0"/>
-      <c r="K74" s="0"/>
-      <c r="L74" s="0"/>
-    </row>
-    <row r="75" spans="1:12">
-      <c r="A75" s="0">
-        <v>12421</v>
-      </c>
-      <c r="B75" s="0">
-        <v>0</v>
-      </c>
-      <c r="C75" s="0">
-        <v>0</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75" s="0">
-        <v>0</v>
-      </c>
-      <c r="F75" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="G75" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H75" s="0">
-        <v>9788522511471</v>
-      </c>
-      <c r="I75" s="0">
-        <v>87.42</v>
-      </c>
-      <c r="J75" s="0"/>
-      <c r="K75" s="0"/>
-      <c r="L75" s="0"/>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="0">
-        <v>12422</v>
-      </c>
-      <c r="B76" s="0">
-        <v>0</v>
-      </c>
-      <c r="C76" s="0">
-        <v>0</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E76" s="0">
-        <v>0</v>
-      </c>
-      <c r="F76" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G76" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H76" s="0">
-        <v>9788575222942</v>
-      </c>
-      <c r="I76" s="0">
-        <v>128.34</v>
-      </c>
-      <c r="J76" s="0"/>
-      <c r="K76" s="0"/>
-      <c r="L76" s="0"/>
-    </row>
-    <row r="77" spans="1:12">
-      <c r="A77" s="0">
-        <v>12423</v>
-      </c>
-      <c r="B77" s="0">
-        <v>0</v>
-      </c>
-      <c r="C77" s="0">
-        <v>0</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="0">
-        <v>0</v>
-      </c>
-      <c r="F77" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="G77" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H77" s="0">
-        <v>9789896685799</v>
-      </c>
-      <c r="I77" s="0">
-        <v>87.42</v>
-      </c>
-      <c r="J77" s="0"/>
-      <c r="K77" s="0"/>
-      <c r="L77" s="0"/>
-    </row>
-    <row r="78" spans="1:12">
-      <c r="A78" s="0">
-        <v>12424</v>
-      </c>
-      <c r="B78" s="0">
-        <v>0</v>
-      </c>
-      <c r="C78" s="0">
-        <v>0</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="0">
-        <v>0</v>
-      </c>
-      <c r="F78" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G78" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H78" s="0">
-        <v>9788582401682</v>
-      </c>
-      <c r="I78" s="0">
-        <v>73.47</v>
-      </c>
-      <c r="J78" s="0"/>
-      <c r="K78" s="0"/>
-      <c r="L78" s="0"/>
-    </row>
-    <row r="79" spans="1:12">
-      <c r="A79" s="0">
-        <v>12425</v>
-      </c>
-      <c r="B79" s="0">
-        <v>0</v>
-      </c>
-      <c r="C79" s="0">
-        <v>0</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" s="0">
-        <v>0</v>
-      </c>
-      <c r="F79" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="G79" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H79" s="0">
-        <v>9788522431472</v>
-      </c>
-      <c r="I79" s="0">
-        <v>308.76</v>
-      </c>
-      <c r="J79" s="0"/>
-      <c r="K79" s="0"/>
-      <c r="L79" s="0"/>
-    </row>
-    <row r="80" spans="1:12">
-      <c r="A80" s="0">
-        <v>12426</v>
-      </c>
-      <c r="B80" s="0">
-        <v>0</v>
-      </c>
-      <c r="C80" s="0">
-        <v>0</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E80" s="0">
-        <v>0</v>
-      </c>
-      <c r="F80" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G80" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H80" s="0">
-        <v>9788539105076</v>
-      </c>
-      <c r="I80" s="0">
-        <v>133.92</v>
-      </c>
-      <c r="J80" s="0"/>
-      <c r="K80" s="0"/>
-      <c r="L80" s="0"/>
-    </row>
-    <row r="81" spans="1:12">
-      <c r="A81" s="0">
-        <v>12427</v>
-      </c>
-      <c r="B81" s="0">
-        <v>0</v>
-      </c>
-      <c r="C81" s="0">
-        <v>0</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="0">
-        <v>0</v>
-      </c>
-      <c r="F81" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="G81" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H81" s="0">
-        <v>9788537010532</v>
-      </c>
-      <c r="I81" s="0">
-        <v>93</v>
-      </c>
-      <c r="J81" s="0"/>
-      <c r="K81" s="0"/>
-      <c r="L81" s="0"/>
-    </row>
-    <row r="82" spans="1:12">
-      <c r="A82" s="0">
-        <v>12428</v>
-      </c>
-      <c r="B82" s="0">
-        <v>0</v>
-      </c>
-      <c r="C82" s="0">
-        <v>1</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" s="0">
-        <v>0</v>
-      </c>
-      <c r="F82" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H82" s="0">
-        <v>9788525054166</v>
-      </c>
-      <c r="I82" s="0">
-        <v>86.49</v>
-      </c>
-      <c r="J82" s="0"/>
-      <c r="K82" s="0"/>
-      <c r="L82" s="0"/>
-    </row>
-    <row r="83" spans="1:12">
-      <c r="A83" s="0">
-        <v>12429</v>
-      </c>
-      <c r="B83" s="0">
-        <v>0</v>
-      </c>
-      <c r="C83" s="0">
-        <v>1</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" s="0">
-        <v>0</v>
-      </c>
-      <c r="F83" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="G83" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H83" s="0">
-        <v>9788539002726</v>
-      </c>
-      <c r="I83" s="0">
-        <v>38.13</v>
-      </c>
-      <c r="J83" s="0"/>
-      <c r="K83" s="0"/>
-      <c r="L83" s="0"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>